<commit_message>
NRL_stats.xslx updated for post TLT projections
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/nrl_stats_scraper_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D890D1C6-24D5-AB4E-AF30-2D40EA077A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B28E6E6-33DF-604D-A1AE-48093CF74E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32820" yWindow="1900" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="29800" yWindow="2500" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -1675,7 +1675,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1809,6 +1809,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2159,7 +2165,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2169,6 +2175,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2548,10 +2556,10 @@
   <dimension ref="A1:K512"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I241" sqref="I241"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,7 +2649,13 @@
         <v>37.11</v>
       </c>
       <c r="H3"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="5">
+        <v>42.3</v>
+      </c>
+      <c r="J3" s="6">
+        <v>5.1899999999999977</v>
+      </c>
+      <c r="K3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -3360,10 +3374,10 @@
       </c>
       <c r="H29"/>
       <c r="I29" s="1">
-        <v>48.9</v>
+        <v>44</v>
       </c>
       <c r="J29" s="1">
-        <v>3.2</v>
+        <v>-2.0700000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -4909,10 +4923,10 @@
       </c>
       <c r="H85"/>
       <c r="I85" s="1">
-        <v>26.3</v>
+        <v>32</v>
       </c>
       <c r="J85" s="1">
-        <v>-2.8</v>
+        <v>2.6700000000000017</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -5671,7 +5685,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -5698,7 +5712,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1</v>
       </c>
@@ -5725,7 +5739,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1</v>
       </c>
@@ -5749,13 +5763,13 @@
       </c>
       <c r="H115"/>
       <c r="I115" s="1">
-        <v>36.9</v>
+        <v>30</v>
       </c>
       <c r="J115" s="1">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-3.4799999999999969</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1</v>
       </c>
@@ -5782,7 +5796,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1</v>
       </c>
@@ -5809,7 +5823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1</v>
       </c>
@@ -5839,7 +5853,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1</v>
       </c>
@@ -5866,7 +5880,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1</v>
       </c>
@@ -5893,7 +5907,7 @@
         <v>-12.4</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1</v>
       </c>
@@ -5920,7 +5934,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1</v>
       </c>
@@ -5947,7 +5961,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1</v>
       </c>
@@ -5974,7 +5988,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1</v>
       </c>
@@ -6001,7 +6015,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1</v>
       </c>
@@ -6021,9 +6035,15 @@
         <v>22.59</v>
       </c>
       <c r="H125"/>
-      <c r="I125" s="1"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I125" s="5">
+        <v>26.7</v>
+      </c>
+      <c r="J125" s="6">
+        <v>4.1099999999999994</v>
+      </c>
+      <c r="K125"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1</v>
       </c>
@@ -6045,7 +6065,7 @@
       <c r="H126"/>
       <c r="I126" s="1"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1</v>
       </c>
@@ -6075,7 +6095,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1</v>
       </c>
@@ -6541,7 +6561,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1</v>
       </c>
@@ -6568,7 +6588,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1</v>
       </c>
@@ -6595,7 +6615,7 @@
         <v>-32.4</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1</v>
       </c>
@@ -6622,7 +6642,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1</v>
       </c>
@@ -6644,7 +6664,7 @@
       <c r="H148"/>
       <c r="I148" s="1"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>1</v>
       </c>
@@ -6674,7 +6694,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1</v>
       </c>
@@ -6701,7 +6721,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1</v>
       </c>
@@ -6723,7 +6743,7 @@
       <c r="H151"/>
       <c r="I151" s="1"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>1</v>
       </c>
@@ -6753,7 +6773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1</v>
       </c>
@@ -6780,7 +6800,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>1</v>
       </c>
@@ -6810,7 +6830,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>1</v>
       </c>
@@ -6837,7 +6857,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1</v>
       </c>
@@ -6867,7 +6887,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>1</v>
       </c>
@@ -6894,7 +6914,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>1</v>
       </c>
@@ -6924,7 +6944,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1</v>
       </c>
@@ -6944,9 +6964,15 @@
         <v>19.93</v>
       </c>
       <c r="H159"/>
-      <c r="I159" s="1"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I159" s="5">
+        <v>28.9</v>
+      </c>
+      <c r="J159" s="6">
+        <v>8.9699999999999989</v>
+      </c>
+      <c r="K159"/>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>1</v>
       </c>
@@ -8804,10 +8830,10 @@
       </c>
       <c r="H228"/>
       <c r="I228" s="1">
-        <v>31.9</v>
+        <v>27</v>
       </c>
       <c r="J228" s="1">
-        <v>10.9</v>
+        <v>5.8900000000000006</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.2">
@@ -10233,10 +10259,10 @@
       </c>
       <c r="H282"/>
       <c r="I282" s="1">
-        <v>40.700000000000003</v>
+        <v>27</v>
       </c>
       <c r="J282" s="1">
-        <v>0.2</v>
+        <v>-13.810000000000002</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.2">
@@ -10691,10 +10717,10 @@
       </c>
       <c r="H300"/>
       <c r="I300" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="J300" s="1">
-        <v>3.4</v>
+        <v>-12.739999999999998</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
@@ -11062,10 +11088,10 @@
       </c>
       <c r="H314"/>
       <c r="I314" s="1">
-        <v>12.8</v>
+        <v>20</v>
       </c>
       <c r="J314" s="1">
-        <v>-9.9</v>
+        <v>-2.8099999999999987</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
@@ -11330,10 +11356,10 @@
       </c>
       <c r="H325"/>
       <c r="I325" s="1">
-        <v>38.299999999999997</v>
+        <v>31</v>
       </c>
       <c r="J325" s="1">
-        <v>-8.6</v>
+        <v>-16.259999999999998</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
@@ -12563,10 +12589,10 @@
       </c>
       <c r="H378"/>
       <c r="I378" s="1">
-        <v>31.9</v>
+        <v>37</v>
       </c>
       <c r="J378" s="1">
-        <v>3.1</v>
+        <v>7.9600000000000009</v>
       </c>
     </row>
     <row r="379" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Google Analytics tracking alongside Hotjar
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B28E6E6-33DF-604D-A1AE-48093CF74E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901AA43-C0FA-2949-AF4B-9CDFF4FFDD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29800" yWindow="2500" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
@@ -2556,10 +2556,10 @@
   <dimension ref="A1:K512"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update NRL_stats.xlsx to remove players no longer included in TLT rd 3
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901AA43-C0FA-2949-AF4B-9CDFF4FFDD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D782DDB1-4CFC-8846-A6ED-D0B811C23F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29800" yWindow="2500" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
@@ -2556,10 +2556,10 @@
   <dimension ref="A1:K512"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="E199" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8009,12 +8009,7 @@
         <v>21.63</v>
       </c>
       <c r="H197"/>
-      <c r="I197" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="J197" s="1">
-        <v>16.3</v>
-      </c>
+      <c r="I197" s="1"/>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198">

</xml_diff>

<commit_message>
update teamlists for round 4
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE56501-7888-2945-84AA-60B578F817B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D726E21-6C8F-014A-A984-3CC746BCA622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29800" yWindow="2500" windowWidth="25400" windowHeight="16360" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="30180" yWindow="3560" windowWidth="25400" windowHeight="16360" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -2559,7 +2559,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:J1048576"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2650,9 +2650,6 @@
       </c>
       <c r="H3"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1">
-        <v>-37.26</v>
-      </c>
       <c r="K3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2676,10 +2673,10 @@
       </c>
       <c r="H4"/>
       <c r="I4" s="1">
-        <v>48.7</v>
+        <v>58.9</v>
       </c>
       <c r="J4" s="1">
-        <v>5.3700000000000045</v>
+        <v>15.57</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2730,10 +2727,10 @@
       </c>
       <c r="H6"/>
       <c r="I6" s="1">
-        <v>44.8</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1">
-        <v>-7.6400000000000006</v>
+        <v>-0.43999999999999773</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2841,9 +2838,6 @@
       </c>
       <c r="H10"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1">
-        <v>-29.7</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -2956,10 +2950,10 @@
       </c>
       <c r="H14"/>
       <c r="I14" s="1">
-        <v>43.5</v>
+        <v>48.2</v>
       </c>
       <c r="J14" s="1">
-        <v>-4.2000000000000028</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3181,10 +3175,10 @@
       </c>
       <c r="H22"/>
       <c r="I22" s="1">
-        <v>56.4</v>
+        <v>52.8</v>
       </c>
       <c r="J22" s="1">
-        <v>13.36</v>
+        <v>9.759999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -3400,10 +3394,10 @@
       </c>
       <c r="H30"/>
       <c r="I30" s="1">
-        <v>59.5</v>
+        <v>58.3</v>
       </c>
       <c r="J30" s="1">
-        <v>5.6499999999999986</v>
+        <v>4.4499999999999957</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -3919,10 +3913,10 @@
       </c>
       <c r="H49"/>
       <c r="I49" s="1">
-        <v>50.2</v>
+        <v>48.5</v>
       </c>
       <c r="J49" s="1">
-        <v>3.0100000000000051</v>
+        <v>1.3100000000000023</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -4027,10 +4021,10 @@
       </c>
       <c r="H53"/>
       <c r="I53" s="1">
-        <v>49.6</v>
+        <v>45.9</v>
       </c>
       <c r="J53" s="1">
-        <v>9.6700000000000017</v>
+        <v>5.9699999999999989</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -4615,10 +4609,10 @@
       </c>
       <c r="H74"/>
       <c r="I74" s="1">
-        <v>51.1</v>
+        <v>49</v>
       </c>
       <c r="J74" s="1">
-        <v>11.100000000000001</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -5089,10 +5083,10 @@
       </c>
       <c r="H91"/>
       <c r="I91" s="1">
-        <v>52.5</v>
+        <v>48.8</v>
       </c>
       <c r="J91" s="1">
-        <v>8.2000000000000028</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -5278,10 +5272,10 @@
       </c>
       <c r="H98"/>
       <c r="I98" s="1">
-        <v>24.8</v>
+        <v>31.5</v>
       </c>
       <c r="J98" s="1">
-        <v>2.3599999999999994</v>
+        <v>9.0599999999999987</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
@@ -5362,10 +5356,10 @@
       </c>
       <c r="H101"/>
       <c r="I101" s="1">
-        <v>34.799999999999997</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="J101" s="1">
-        <v>1.4699999999999989</v>
+        <v>5.3700000000000045</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
@@ -5563,9 +5557,6 @@
       </c>
       <c r="H108"/>
       <c r="I108" s="1"/>
-      <c r="J108" s="1">
-        <v>-33.479999999999997</v>
-      </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
@@ -6084,9 +6075,6 @@
       </c>
       <c r="H127"/>
       <c r="I127" s="1"/>
-      <c r="J127" s="1">
-        <v>-38</v>
-      </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
@@ -6306,12 +6294,7 @@
         <v>33.479999999999997</v>
       </c>
       <c r="H135"/>
-      <c r="I135" s="1">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="J135" s="1">
-        <v>2.220000000000006</v>
-      </c>
+      <c r="I135" s="1"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136">
@@ -6418,10 +6401,10 @@
       </c>
       <c r="H139"/>
       <c r="I139" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J139" s="1">
-        <v>-32.78</v>
+        <v>-29.78</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
@@ -6472,9 +6455,6 @@
       </c>
       <c r="H141"/>
       <c r="I141" s="1"/>
-      <c r="J141" s="1">
-        <v>-29.56</v>
-      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142">
@@ -6662,9 +6642,6 @@
       </c>
       <c r="H148"/>
       <c r="I148" s="1"/>
-      <c r="J148" s="1">
-        <v>-36.96</v>
-      </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
@@ -6744,9 +6721,6 @@
       </c>
       <c r="H151"/>
       <c r="I151" s="1"/>
-      <c r="J151" s="1">
-        <v>-33.56</v>
-      </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
@@ -7346,10 +7320,10 @@
       </c>
       <c r="H173"/>
       <c r="I173" s="1">
-        <v>43.5</v>
+        <v>42.2</v>
       </c>
       <c r="J173" s="1">
-        <v>3.5700000000000003</v>
+        <v>2.2700000000000031</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
@@ -7433,10 +7407,10 @@
       </c>
       <c r="H176"/>
       <c r="I176" s="1">
-        <v>39.5</v>
+        <v>37.9</v>
       </c>
       <c r="J176" s="1">
-        <v>10.309999999999999</v>
+        <v>8.7099999999999973</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
@@ -7517,9 +7491,6 @@
       </c>
       <c r="H179"/>
       <c r="I179" s="1"/>
-      <c r="J179" s="1">
-        <v>-33.85</v>
-      </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180">
@@ -7767,10 +7738,10 @@
       </c>
       <c r="H188"/>
       <c r="I188" s="1">
-        <v>49</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="J188" s="1">
-        <v>4.93</v>
+        <v>-3.7700000000000031</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
@@ -8154,9 +8125,6 @@
       </c>
       <c r="H202"/>
       <c r="I202" s="1"/>
-      <c r="J202" s="1">
-        <v>-20.74</v>
-      </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203">
@@ -8287,9 +8255,6 @@
       </c>
       <c r="H207"/>
       <c r="I207" s="1"/>
-      <c r="J207" s="1">
-        <v>-28.74</v>
-      </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208">
@@ -8393,9 +8358,6 @@
       </c>
       <c r="H211"/>
       <c r="I211" s="1"/>
-      <c r="J211" s="1">
-        <v>-21.63</v>
-      </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212">
@@ -8586,10 +8548,10 @@
       </c>
       <c r="H218"/>
       <c r="I218" s="1">
-        <v>31.5</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="J218" s="1">
-        <v>10.829999999999998</v>
+        <v>12.629999999999995</v>
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.2">
@@ -8751,9 +8713,6 @@
       </c>
       <c r="H224"/>
       <c r="I224" s="1"/>
-      <c r="J224" s="1">
-        <v>-22.74</v>
-      </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225">
@@ -8803,10 +8762,10 @@
       </c>
       <c r="H226"/>
       <c r="I226" s="1">
-        <v>41.9</v>
+        <v>35.6</v>
       </c>
       <c r="J226" s="1">
-        <v>10.049999999999997</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.2">
@@ -8884,10 +8843,10 @@
       </c>
       <c r="H229"/>
       <c r="I229" s="1">
-        <v>42.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="J229" s="1">
-        <v>8.2600000000000051</v>
+        <v>4.2600000000000051</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.2">
@@ -8938,9 +8897,6 @@
       </c>
       <c r="H231"/>
       <c r="I231" s="1"/>
-      <c r="J231" s="1">
-        <v>-28</v>
-      </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232">
@@ -9128,9 +9084,6 @@
       </c>
       <c r="H238"/>
       <c r="I238" s="1"/>
-      <c r="J238" s="1">
-        <v>-19.93</v>
-      </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239">
@@ -9153,9 +9106,6 @@
       </c>
       <c r="H239"/>
       <c r="I239" s="1"/>
-      <c r="J239" s="1">
-        <v>-19.190000000000001</v>
-      </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240">
@@ -9178,10 +9128,10 @@
       </c>
       <c r="H240"/>
       <c r="I240" s="1">
-        <v>31</v>
+        <v>30.6</v>
       </c>
       <c r="J240" s="1">
-        <v>-1.3699999999999974</v>
+        <v>-1.769999999999996</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.2">
@@ -9235,9 +9185,6 @@
       </c>
       <c r="H242"/>
       <c r="I242" s="1"/>
-      <c r="J242" s="1">
-        <v>-29.26</v>
-      </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243">
@@ -9287,10 +9234,10 @@
       </c>
       <c r="H244"/>
       <c r="I244" s="1">
-        <v>29.5</v>
+        <v>27.7</v>
       </c>
       <c r="J244" s="1">
-        <v>1.8000000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.2">
@@ -9314,10 +9261,10 @@
       </c>
       <c r="H245"/>
       <c r="I245" s="1">
-        <v>35.700000000000003</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="J245" s="1">
-        <v>7.4000000000000021</v>
+        <v>9.9999999999999964</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.2">
@@ -9341,10 +9288,10 @@
       </c>
       <c r="H246"/>
       <c r="I246" s="1">
-        <v>45</v>
+        <v>47.4</v>
       </c>
       <c r="J246" s="1">
-        <v>2.7800000000000011</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.2">
@@ -9422,9 +9369,6 @@
       </c>
       <c r="H249"/>
       <c r="I249" s="1"/>
-      <c r="J249" s="1">
-        <v>-22.52</v>
-      </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250">
@@ -9621,9 +9565,6 @@
       </c>
       <c r="H256"/>
       <c r="I256" s="1"/>
-      <c r="J256" s="1">
-        <v>-25.78</v>
-      </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257">
@@ -9706,9 +9647,6 @@
       </c>
       <c r="H259"/>
       <c r="I259" s="1"/>
-      <c r="J259" s="1">
-        <v>-29.26</v>
-      </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260">
@@ -9731,9 +9669,6 @@
       </c>
       <c r="H260"/>
       <c r="I260" s="1"/>
-      <c r="J260" s="1">
-        <v>-21.85</v>
-      </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261">
@@ -9756,9 +9691,6 @@
       </c>
       <c r="H261"/>
       <c r="I261" s="1"/>
-      <c r="J261" s="1">
-        <v>-20.3</v>
-      </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262">
@@ -9781,9 +9713,6 @@
       </c>
       <c r="H262"/>
       <c r="I262" s="1"/>
-      <c r="J262" s="1">
-        <v>-26.74</v>
-      </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263">
@@ -9863,9 +9792,6 @@
       </c>
       <c r="H265"/>
       <c r="I265" s="1"/>
-      <c r="J265" s="1">
-        <v>-27.56</v>
-      </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266">
@@ -9888,9 +9814,6 @@
       </c>
       <c r="H266"/>
       <c r="I266" s="1"/>
-      <c r="J266" s="1">
-        <v>-18.96</v>
-      </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267">
@@ -9913,9 +9836,6 @@
       </c>
       <c r="H267"/>
       <c r="I267" s="1"/>
-      <c r="J267" s="1">
-        <v>-21.48</v>
-      </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268">
@@ -10106,9 +10026,6 @@
       </c>
       <c r="H274"/>
       <c r="I274" s="1"/>
-      <c r="J274" s="1">
-        <v>-21.63</v>
-      </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275">
@@ -10271,12 +10188,7 @@
         <v>30.07</v>
       </c>
       <c r="H280"/>
-      <c r="I280" s="1">
-        <v>31.5</v>
-      </c>
-      <c r="J280" s="1">
-        <v>1.4299999999999997</v>
-      </c>
+      <c r="I280" s="1"/>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281">
@@ -10326,9 +10238,6 @@
       </c>
       <c r="H282"/>
       <c r="I282" s="1"/>
-      <c r="J282" s="1">
-        <v>-19.11</v>
-      </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283">
@@ -10378,10 +10287,10 @@
       </c>
       <c r="H284"/>
       <c r="I284" s="1">
-        <v>45.8</v>
+        <v>41.9</v>
       </c>
       <c r="J284" s="1">
-        <v>12.759999999999998</v>
+        <v>8.86</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.2">
@@ -10459,10 +10368,10 @@
       </c>
       <c r="H287"/>
       <c r="I287" s="1">
-        <v>11.7</v>
+        <v>15</v>
       </c>
       <c r="J287" s="1">
-        <v>-6.3000000000000007</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.2">
@@ -10513,10 +10422,10 @@
       </c>
       <c r="H289"/>
       <c r="I289" s="1">
-        <v>24.2</v>
+        <v>23.5</v>
       </c>
       <c r="J289" s="1">
-        <v>5.16</v>
+        <v>4.4600000000000009</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.2">
@@ -10567,9 +10476,6 @@
       </c>
       <c r="H291"/>
       <c r="I291" s="1"/>
-      <c r="J291" s="1">
-        <v>-21.93</v>
-      </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292">
@@ -10621,12 +10527,7 @@
         <v>31.63</v>
       </c>
       <c r="H293"/>
-      <c r="I293" s="1">
-        <v>21.6</v>
-      </c>
-      <c r="J293" s="1">
-        <v>-10.029999999999998</v>
-      </c>
+      <c r="I293" s="1"/>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294">
@@ -10649,9 +10550,6 @@
       </c>
       <c r="H294"/>
       <c r="I294" s="1"/>
-      <c r="J294" s="1">
-        <v>-25.26</v>
-      </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295">
@@ -10704,9 +10602,6 @@
       </c>
       <c r="H296"/>
       <c r="I296" s="1"/>
-      <c r="J296" s="1">
-        <v>-28.74</v>
-      </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297">
@@ -10729,9 +10624,6 @@
       </c>
       <c r="H297"/>
       <c r="I297" s="1"/>
-      <c r="J297" s="1">
-        <v>-26.96</v>
-      </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298">
@@ -10754,9 +10646,6 @@
       </c>
       <c r="H298"/>
       <c r="I298" s="1"/>
-      <c r="J298" s="1">
-        <v>-18.59</v>
-      </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299">
@@ -10782,9 +10671,6 @@
       </c>
       <c r="H299"/>
       <c r="I299" s="1"/>
-      <c r="J299" s="1">
-        <v>-26.81</v>
-      </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300">
@@ -10807,9 +10693,6 @@
       </c>
       <c r="H300"/>
       <c r="I300" s="1"/>
-      <c r="J300" s="1">
-        <v>-24.07</v>
-      </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301">
@@ -10832,9 +10715,6 @@
       </c>
       <c r="H301"/>
       <c r="I301" s="1"/>
-      <c r="J301" s="1">
-        <v>-22.44</v>
-      </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302">
@@ -10857,9 +10737,6 @@
       </c>
       <c r="H302"/>
       <c r="I302" s="1"/>
-      <c r="J302" s="1">
-        <v>-17.11</v>
-      </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303">
@@ -10882,9 +10759,6 @@
       </c>
       <c r="H303"/>
       <c r="I303" s="1"/>
-      <c r="J303" s="1">
-        <v>-18.07</v>
-      </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304">
@@ -10907,9 +10781,6 @@
       </c>
       <c r="H304"/>
       <c r="I304" s="1"/>
-      <c r="J304" s="1">
-        <v>-17.41</v>
-      </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305">
@@ -10932,9 +10803,6 @@
       </c>
       <c r="H305"/>
       <c r="I305" s="1"/>
-      <c r="J305" s="1">
-        <v>-29.93</v>
-      </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306">
@@ -10957,9 +10825,6 @@
       </c>
       <c r="H306"/>
       <c r="I306" s="1"/>
-      <c r="J306" s="1">
-        <v>-24.44</v>
-      </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307">
@@ -10982,9 +10847,6 @@
       </c>
       <c r="H307"/>
       <c r="I307" s="1"/>
-      <c r="J307" s="1">
-        <v>-23.33</v>
-      </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308">
@@ -11064,9 +10926,6 @@
       </c>
       <c r="H310"/>
       <c r="I310" s="1"/>
-      <c r="J310" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311">
@@ -11149,9 +11008,6 @@
       </c>
       <c r="H313"/>
       <c r="I313" s="1"/>
-      <c r="J313" s="1">
-        <v>-18.22</v>
-      </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314">
@@ -11174,9 +11030,6 @@
       </c>
       <c r="H314"/>
       <c r="I314" s="1"/>
-      <c r="J314" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315">
@@ -11201,9 +11054,11 @@
         <v>22.81</v>
       </c>
       <c r="H315"/>
-      <c r="I315" s="1"/>
+      <c r="I315" s="1">
+        <v>26.1</v>
+      </c>
       <c r="J315" s="1">
-        <v>-22.81</v>
+        <v>3.2900000000000027</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.2">
@@ -11317,9 +11172,6 @@
       </c>
       <c r="H319"/>
       <c r="I319" s="1"/>
-      <c r="J319" s="1">
-        <v>-24.81</v>
-      </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320">
@@ -11341,12 +11193,7 @@
         <v>17.04</v>
       </c>
       <c r="H320"/>
-      <c r="I320" s="1">
-        <v>19</v>
-      </c>
-      <c r="J320" s="1">
-        <v>1.9600000000000009</v>
-      </c>
+      <c r="I320" s="1"/>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321">
@@ -11369,9 +11216,6 @@
       </c>
       <c r="H321"/>
       <c r="I321" s="1"/>
-      <c r="J321" s="1">
-        <v>-24.96</v>
-      </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322">
@@ -11448,9 +11292,6 @@
       </c>
       <c r="H324"/>
       <c r="I324" s="1"/>
-      <c r="J324" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325">
@@ -11473,9 +11314,6 @@
       </c>
       <c r="H325"/>
       <c r="I325" s="1"/>
-      <c r="J325" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326">
@@ -11585,9 +11423,6 @@
       </c>
       <c r="H329"/>
       <c r="I329" s="1"/>
-      <c r="J329" s="1">
-        <v>-20.67</v>
-      </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330">
@@ -11640,9 +11475,6 @@
       </c>
       <c r="H331"/>
       <c r="I331" s="1"/>
-      <c r="J331" s="1">
-        <v>-27.93</v>
-      </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332">
@@ -11695,9 +11527,6 @@
       </c>
       <c r="H333"/>
       <c r="I333" s="1"/>
-      <c r="J333" s="1">
-        <v>-17.329999999999998</v>
-      </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334">
@@ -11720,9 +11549,6 @@
       </c>
       <c r="H334"/>
       <c r="I334" s="1"/>
-      <c r="J334" s="1">
-        <v>-17.190000000000001</v>
-      </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335">
@@ -11772,9 +11598,6 @@
       </c>
       <c r="H336"/>
       <c r="I336" s="1"/>
-      <c r="J336" s="1">
-        <v>-54.59</v>
-      </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337">
@@ -11797,9 +11620,6 @@
       </c>
       <c r="H337"/>
       <c r="I337" s="1"/>
-      <c r="J337" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338">
@@ -11849,9 +11669,6 @@
       </c>
       <c r="H339"/>
       <c r="I339" s="1"/>
-      <c r="J339" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340">
@@ -11874,9 +11691,6 @@
       </c>
       <c r="H340"/>
       <c r="I340" s="1"/>
-      <c r="J340" s="1">
-        <v>-49.26</v>
-      </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341">
@@ -11926,9 +11740,6 @@
       </c>
       <c r="H342"/>
       <c r="I342" s="1"/>
-      <c r="J342" s="1">
-        <v>-47.7</v>
-      </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343">
@@ -11951,9 +11762,6 @@
       </c>
       <c r="H343"/>
       <c r="I343" s="1"/>
-      <c r="J343" s="1">
-        <v>-47.56</v>
-      </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344">
@@ -12039,9 +11847,6 @@
       </c>
       <c r="H346"/>
       <c r="I346" s="1"/>
-      <c r="J346" s="1">
-        <v>-45.63</v>
-      </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347">
@@ -12064,9 +11869,6 @@
       </c>
       <c r="H347"/>
       <c r="I347" s="1"/>
-      <c r="J347" s="1">
-        <v>-43.7</v>
-      </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348">
@@ -12089,9 +11891,6 @@
       </c>
       <c r="H348"/>
       <c r="I348" s="1"/>
-      <c r="J348" s="1">
-        <v>-40.74</v>
-      </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349">
@@ -12114,9 +11913,6 @@
       </c>
       <c r="H349"/>
       <c r="I349" s="1"/>
-      <c r="J349" s="1">
-        <v>-42.67</v>
-      </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350">
@@ -12139,9 +11935,6 @@
       </c>
       <c r="H350"/>
       <c r="I350" s="1"/>
-      <c r="J350" s="1">
-        <v>-42.44</v>
-      </c>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351">
@@ -12167,9 +11960,6 @@
       </c>
       <c r="H351"/>
       <c r="I351" s="1"/>
-      <c r="J351" s="1">
-        <v>-42</v>
-      </c>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352">
@@ -12192,9 +11982,6 @@
       </c>
       <c r="H352"/>
       <c r="I352" s="1"/>
-      <c r="J352" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353">
@@ -12217,9 +12004,6 @@
       </c>
       <c r="H353"/>
       <c r="I353" s="1"/>
-      <c r="J353" s="1">
-        <v>-38.89</v>
-      </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354">
@@ -12242,9 +12026,6 @@
       </c>
       <c r="H354"/>
       <c r="I354" s="1"/>
-      <c r="J354" s="1">
-        <v>-37.700000000000003</v>
-      </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355">
@@ -12267,9 +12048,6 @@
       </c>
       <c r="H355"/>
       <c r="I355" s="1"/>
-      <c r="J355" s="1">
-        <v>-33.33</v>
-      </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356">
@@ -12292,9 +12070,6 @@
       </c>
       <c r="H356"/>
       <c r="I356" s="1"/>
-      <c r="J356" s="1">
-        <v>-37.19</v>
-      </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357">
@@ -12344,9 +12119,6 @@
       </c>
       <c r="H358"/>
       <c r="I358" s="1"/>
-      <c r="J358" s="1">
-        <v>-36.81</v>
-      </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359">
@@ -12369,9 +12141,6 @@
       </c>
       <c r="H359"/>
       <c r="I359" s="1"/>
-      <c r="J359" s="1">
-        <v>-36.369999999999997</v>
-      </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360">
@@ -12394,9 +12163,6 @@
       </c>
       <c r="H360"/>
       <c r="I360" s="1"/>
-      <c r="J360" s="1">
-        <v>-35.33</v>
-      </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361">
@@ -12419,9 +12185,6 @@
       </c>
       <c r="H361"/>
       <c r="I361" s="1"/>
-      <c r="J361" s="1">
-        <v>-29.63</v>
-      </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362">
@@ -12444,9 +12207,6 @@
       </c>
       <c r="H362"/>
       <c r="I362" s="1"/>
-      <c r="J362" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363">
@@ -12472,9 +12232,6 @@
       </c>
       <c r="H363"/>
       <c r="I363" s="1"/>
-      <c r="J363" s="1">
-        <v>-34.44</v>
-      </c>
     </row>
     <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364">
@@ -12500,9 +12257,6 @@
       </c>
       <c r="H364"/>
       <c r="I364" s="1"/>
-      <c r="J364" s="1">
-        <v>-34.44</v>
-      </c>
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365">
@@ -12525,9 +12279,6 @@
       </c>
       <c r="H365"/>
       <c r="I365" s="1"/>
-      <c r="J365" s="1">
-        <v>-33.78</v>
-      </c>
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366">
@@ -12550,9 +12301,6 @@
       </c>
       <c r="H366"/>
       <c r="I366" s="1"/>
-      <c r="J366" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367">
@@ -12575,9 +12323,6 @@
       </c>
       <c r="H367"/>
       <c r="I367" s="1"/>
-      <c r="J367" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368">
@@ -12600,9 +12345,6 @@
       </c>
       <c r="H368"/>
       <c r="I368" s="1"/>
-      <c r="J368" s="1">
-        <v>-33.479999999999997</v>
-      </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369">
@@ -12625,9 +12367,6 @@
       </c>
       <c r="H369"/>
       <c r="I369" s="1"/>
-      <c r="J369" s="1">
-        <v>-33.33</v>
-      </c>
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370">
@@ -12653,9 +12392,6 @@
       </c>
       <c r="H370"/>
       <c r="I370" s="1"/>
-      <c r="J370" s="1">
-        <v>-33.26</v>
-      </c>
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371">
@@ -12678,9 +12414,6 @@
       </c>
       <c r="H371"/>
       <c r="I371" s="1"/>
-      <c r="J371" s="1">
-        <v>-32.81</v>
-      </c>
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372">
@@ -12703,9 +12436,6 @@
       </c>
       <c r="H372"/>
       <c r="I372" s="1"/>
-      <c r="J372" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373">
@@ -12728,9 +12458,6 @@
       </c>
       <c r="H373"/>
       <c r="I373" s="1"/>
-      <c r="J373" s="1">
-        <v>-32.67</v>
-      </c>
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374">
@@ -12752,9 +12479,11 @@
         <v>32.520000000000003</v>
       </c>
       <c r="H374"/>
-      <c r="I374" s="1"/>
+      <c r="I374" s="1">
+        <v>39.1</v>
+      </c>
       <c r="J374" s="1">
-        <v>-32.520000000000003</v>
+        <v>6.5799999999999983</v>
       </c>
     </row>
     <row r="375" spans="1:10" x14ac:dyDescent="0.2">
@@ -12778,9 +12507,6 @@
       </c>
       <c r="H375"/>
       <c r="I375" s="1"/>
-      <c r="J375" s="1">
-        <v>-32.07</v>
-      </c>
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376">
@@ -12805,12 +12531,7 @@
         <v>31.93</v>
       </c>
       <c r="H376"/>
-      <c r="I376" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="J376" s="1">
-        <v>3.6700000000000017</v>
-      </c>
+      <c r="I376" s="1"/>
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377">
@@ -12833,9 +12554,6 @@
       </c>
       <c r="H377"/>
       <c r="I377" s="1"/>
-      <c r="J377" s="1">
-        <v>-31.93</v>
-      </c>
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A378">
@@ -12858,9 +12576,6 @@
       </c>
       <c r="H378"/>
       <c r="I378" s="1"/>
-      <c r="J378" s="1">
-        <v>-31.63</v>
-      </c>
     </row>
     <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379">
@@ -12883,9 +12598,6 @@
       </c>
       <c r="H379"/>
       <c r="I379" s="1"/>
-      <c r="J379" s="1">
-        <v>-33.33</v>
-      </c>
     </row>
     <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380">
@@ -12911,9 +12623,6 @@
       </c>
       <c r="H380"/>
       <c r="I380" s="1"/>
-      <c r="J380" s="1">
-        <v>-31.19</v>
-      </c>
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381">
@@ -12963,9 +12672,6 @@
       </c>
       <c r="H382"/>
       <c r="I382" s="1"/>
-      <c r="J382" s="1">
-        <v>-30.81</v>
-      </c>
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383">
@@ -12988,9 +12694,6 @@
       </c>
       <c r="H383"/>
       <c r="I383" s="1"/>
-      <c r="J383" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384">
@@ -13012,12 +12715,14 @@
         <v>30.59</v>
       </c>
       <c r="H384"/>
-      <c r="I384" s="1"/>
+      <c r="I384" s="1">
+        <v>26.4</v>
+      </c>
       <c r="J384" s="1">
-        <v>-30.59</v>
-      </c>
-    </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-4.1900000000000013</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>1</v>
       </c>
@@ -13038,11 +12743,8 @@
       </c>
       <c r="H385"/>
       <c r="I385" s="1"/>
-      <c r="J385" s="1">
-        <v>-30.3</v>
-      </c>
-    </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>1</v>
       </c>
@@ -13063,11 +12765,8 @@
       </c>
       <c r="H386"/>
       <c r="I386" s="1"/>
-      <c r="J386" s="1">
-        <v>-30.22</v>
-      </c>
-    </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>1</v>
       </c>
@@ -13091,11 +12790,8 @@
       </c>
       <c r="H387"/>
       <c r="I387" s="1"/>
-      <c r="J387" s="1">
-        <v>-25.93</v>
-      </c>
-    </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>1</v>
       </c>
@@ -13116,11 +12812,8 @@
       </c>
       <c r="H388"/>
       <c r="I388" s="1"/>
-      <c r="J388" s="1">
-        <v>-29.7</v>
-      </c>
-    </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>1</v>
       </c>
@@ -13141,11 +12834,8 @@
       </c>
       <c r="H389"/>
       <c r="I389" s="1"/>
-      <c r="J389" s="1">
-        <v>-29.48</v>
-      </c>
-    </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>1</v>
       </c>
@@ -13166,11 +12856,8 @@
       </c>
       <c r="H390"/>
       <c r="I390" s="1"/>
-      <c r="J390" s="1">
-        <v>-29.04</v>
-      </c>
-    </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>1</v>
       </c>
@@ -13191,11 +12878,8 @@
       </c>
       <c r="H391"/>
       <c r="I391" s="1"/>
-      <c r="J391" s="1">
-        <v>-29.04</v>
-      </c>
-    </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>1</v>
       </c>
@@ -13216,11 +12900,8 @@
       </c>
       <c r="H392"/>
       <c r="I392" s="1"/>
-      <c r="J392" s="1">
-        <v>-28.89</v>
-      </c>
-    </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>1</v>
       </c>
@@ -13241,11 +12922,8 @@
       </c>
       <c r="H393"/>
       <c r="I393" s="1"/>
-      <c r="J393" s="1">
-        <v>-28.81</v>
-      </c>
-    </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="394" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>1</v>
       </c>
@@ -13266,11 +12944,8 @@
       </c>
       <c r="H394"/>
       <c r="I394" s="1"/>
-      <c r="J394" s="1">
-        <v>-25.93</v>
-      </c>
-    </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="395" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>1</v>
       </c>
@@ -13291,11 +12966,8 @@
       </c>
       <c r="H395"/>
       <c r="I395" s="1"/>
-      <c r="J395" s="1">
-        <v>-25.93</v>
-      </c>
-    </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>1</v>
       </c>
@@ -13316,11 +12988,8 @@
       </c>
       <c r="H396"/>
       <c r="I396" s="1"/>
-      <c r="J396" s="1">
-        <v>-28.22</v>
-      </c>
-    </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>1</v>
       </c>
@@ -13344,11 +13013,8 @@
       </c>
       <c r="H397"/>
       <c r="I397" s="1"/>
-      <c r="J397" s="1">
-        <v>-28.3</v>
-      </c>
-    </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>1</v>
       </c>
@@ -13369,11 +13035,8 @@
       </c>
       <c r="H398"/>
       <c r="I398" s="1"/>
-      <c r="J398" s="1">
-        <v>-28.22</v>
-      </c>
-    </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>1</v>
       </c>
@@ -13394,11 +13057,8 @@
       </c>
       <c r="H399"/>
       <c r="I399" s="1"/>
-      <c r="J399" s="1">
-        <v>-27.93</v>
-      </c>
-    </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>1</v>
       </c>
@@ -13422,9 +13082,6 @@
       </c>
       <c r="H400"/>
       <c r="I400" s="1"/>
-      <c r="J400" s="1">
-        <v>-27.78</v>
-      </c>
     </row>
     <row r="401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A401">
@@ -13447,9 +13104,6 @@
       </c>
       <c r="H401"/>
       <c r="I401" s="1"/>
-      <c r="J401" s="1">
-        <v>-27.78</v>
-      </c>
     </row>
     <row r="402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A402">
@@ -13472,9 +13126,6 @@
       </c>
       <c r="H402"/>
       <c r="I402" s="1"/>
-      <c r="J402" s="1">
-        <v>-27.7</v>
-      </c>
     </row>
     <row r="403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A403">
@@ -13500,9 +13151,6 @@
       </c>
       <c r="H403"/>
       <c r="I403" s="1"/>
-      <c r="J403" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A404">
@@ -13552,9 +13200,6 @@
       </c>
       <c r="H405"/>
       <c r="I405" s="1"/>
-      <c r="J405" s="1">
-        <v>-24.22</v>
-      </c>
     </row>
     <row r="406" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A406">
@@ -13577,9 +13222,6 @@
       </c>
       <c r="H406"/>
       <c r="I406" s="1"/>
-      <c r="J406" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A407">
@@ -13602,9 +13244,6 @@
       </c>
       <c r="H407"/>
       <c r="I407" s="1"/>
-      <c r="J407" s="1">
-        <v>-25.48</v>
-      </c>
     </row>
     <row r="408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A408">
@@ -13630,9 +13269,6 @@
       </c>
       <c r="H408"/>
       <c r="I408" s="1"/>
-      <c r="J408" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A409">
@@ -13655,9 +13291,6 @@
       </c>
       <c r="H409"/>
       <c r="I409" s="1"/>
-      <c r="J409" s="1">
-        <v>-24.96</v>
-      </c>
     </row>
     <row r="410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A410">
@@ -13680,9 +13313,6 @@
       </c>
       <c r="H410"/>
       <c r="I410" s="1"/>
-      <c r="J410" s="1">
-        <v>-24.89</v>
-      </c>
     </row>
     <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411">
@@ -13705,9 +13335,6 @@
       </c>
       <c r="H411"/>
       <c r="I411" s="1"/>
-      <c r="J411" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A412">
@@ -13730,9 +13357,6 @@
       </c>
       <c r="H412"/>
       <c r="I412" s="1"/>
-      <c r="J412" s="1">
-        <v>-24.44</v>
-      </c>
     </row>
     <row r="413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A413">
@@ -13755,9 +13379,6 @@
       </c>
       <c r="H413"/>
       <c r="I413" s="1"/>
-      <c r="J413" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A414">
@@ -13780,9 +13401,6 @@
       </c>
       <c r="H414"/>
       <c r="I414" s="1"/>
-      <c r="J414" s="1">
-        <v>-23.56</v>
-      </c>
     </row>
     <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A415">
@@ -13805,9 +13423,6 @@
       </c>
       <c r="H415"/>
       <c r="I415" s="1"/>
-      <c r="J415" s="1">
-        <v>-23.48</v>
-      </c>
     </row>
     <row r="416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A416">
@@ -13830,9 +13445,6 @@
       </c>
       <c r="H416"/>
       <c r="I416" s="1"/>
-      <c r="J416" s="1">
-        <v>-23.26</v>
-      </c>
     </row>
     <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417">
@@ -13855,9 +13467,6 @@
       </c>
       <c r="H417"/>
       <c r="I417" s="1"/>
-      <c r="J417" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418">
@@ -13880,9 +13489,6 @@
       </c>
       <c r="H418"/>
       <c r="I418" s="1"/>
-      <c r="J418" s="1">
-        <v>-22.3</v>
-      </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419">
@@ -13905,9 +13511,6 @@
       </c>
       <c r="H419"/>
       <c r="I419" s="1"/>
-      <c r="J419" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420">
@@ -13930,9 +13533,6 @@
       </c>
       <c r="H420"/>
       <c r="I420" s="1"/>
-      <c r="J420" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421">
@@ -13955,9 +13555,6 @@
       </c>
       <c r="H421"/>
       <c r="I421" s="1"/>
-      <c r="J421" s="1">
-        <v>-21.19</v>
-      </c>
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422">
@@ -13980,9 +13577,6 @@
       </c>
       <c r="H422"/>
       <c r="I422" s="1"/>
-      <c r="J422" s="1">
-        <v>-21.04</v>
-      </c>
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423">
@@ -14035,9 +13629,6 @@
       </c>
       <c r="H424"/>
       <c r="I424" s="1"/>
-      <c r="J424" s="1">
-        <v>-20.52</v>
-      </c>
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425">
@@ -14060,9 +13651,6 @@
       </c>
       <c r="H425"/>
       <c r="I425" s="1"/>
-      <c r="J425" s="1">
-        <v>-20.37</v>
-      </c>
     </row>
     <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426">
@@ -14085,9 +13673,6 @@
       </c>
       <c r="H426"/>
       <c r="I426" s="1"/>
-      <c r="J426" s="1">
-        <v>-20.3</v>
-      </c>
     </row>
     <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427">
@@ -14110,9 +13695,6 @@
       </c>
       <c r="H427"/>
       <c r="I427" s="1"/>
-      <c r="J427" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428">
@@ -14135,9 +13717,6 @@
       </c>
       <c r="H428"/>
       <c r="I428" s="1"/>
-      <c r="J428" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429">
@@ -14160,9 +13739,6 @@
       </c>
       <c r="H429"/>
       <c r="I429" s="1"/>
-      <c r="J429" s="1">
-        <v>-20</v>
-      </c>
     </row>
     <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430">
@@ -14185,9 +13761,6 @@
       </c>
       <c r="H430"/>
       <c r="I430" s="1"/>
-      <c r="J430" s="1">
-        <v>-18.96</v>
-      </c>
     </row>
     <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431">
@@ -14210,9 +13783,6 @@
       </c>
       <c r="H431"/>
       <c r="I431" s="1"/>
-      <c r="J431" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432">
@@ -14235,11 +13805,8 @@
       </c>
       <c r="H432"/>
       <c r="I432" s="1"/>
-      <c r="J432" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>1</v>
       </c>
@@ -14260,11 +13827,8 @@
       </c>
       <c r="H433"/>
       <c r="I433" s="1"/>
-      <c r="J433" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>1</v>
       </c>
@@ -14285,11 +13849,8 @@
       </c>
       <c r="H434"/>
       <c r="I434" s="1"/>
-      <c r="J434" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>1</v>
       </c>
@@ -14310,11 +13871,8 @@
       </c>
       <c r="H435"/>
       <c r="I435" s="1"/>
-      <c r="J435" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>1</v>
       </c>
@@ -14335,11 +13893,8 @@
       </c>
       <c r="H436"/>
       <c r="I436" s="1"/>
-      <c r="J436" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>1</v>
       </c>
@@ -14360,11 +13915,8 @@
       </c>
       <c r="H437"/>
       <c r="I437" s="1"/>
-      <c r="J437" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>1</v>
       </c>
@@ -14385,11 +13937,8 @@
       </c>
       <c r="H438"/>
       <c r="I438" s="1"/>
-      <c r="J438" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>1</v>
       </c>
@@ -14410,11 +13959,8 @@
       </c>
       <c r="H439"/>
       <c r="I439" s="1"/>
-      <c r="J439" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>1</v>
       </c>
@@ -14435,11 +13981,8 @@
       </c>
       <c r="H440"/>
       <c r="I440" s="1"/>
-      <c r="J440" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>1</v>
       </c>
@@ -14460,11 +14003,8 @@
       </c>
       <c r="H441"/>
       <c r="I441" s="1"/>
-      <c r="J441" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>1</v>
       </c>
@@ -14485,11 +14025,8 @@
       </c>
       <c r="H442"/>
       <c r="I442" s="1"/>
-      <c r="J442" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>1</v>
       </c>
@@ -14510,11 +14047,8 @@
       </c>
       <c r="H443"/>
       <c r="I443" s="1"/>
-      <c r="J443" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>1</v>
       </c>
@@ -14535,11 +14069,8 @@
       </c>
       <c r="H444"/>
       <c r="I444" s="1"/>
-      <c r="J444" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>1</v>
       </c>
@@ -14560,11 +14091,8 @@
       </c>
       <c r="H445"/>
       <c r="I445" s="1"/>
-      <c r="J445" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>1</v>
       </c>
@@ -14585,11 +14113,8 @@
       </c>
       <c r="H446"/>
       <c r="I446" s="1"/>
-      <c r="J446" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>1</v>
       </c>
@@ -14610,11 +14135,8 @@
       </c>
       <c r="H447"/>
       <c r="I447" s="1"/>
-      <c r="J447" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>1</v>
       </c>
@@ -14635,9 +14157,6 @@
       </c>
       <c r="H448"/>
       <c r="I448" s="1"/>
-      <c r="J448" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A449">
@@ -14660,9 +14179,6 @@
       </c>
       <c r="H449"/>
       <c r="I449" s="1"/>
-      <c r="J449" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A450">
@@ -14685,9 +14201,6 @@
       </c>
       <c r="H450"/>
       <c r="I450" s="1"/>
-      <c r="J450" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="451" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A451">
@@ -14710,9 +14223,6 @@
       </c>
       <c r="H451"/>
       <c r="I451" s="1"/>
-      <c r="J451" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="452" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A452">
@@ -14735,9 +14245,6 @@
       </c>
       <c r="H452"/>
       <c r="I452" s="1"/>
-      <c r="J452" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A453">
@@ -14760,9 +14267,6 @@
       </c>
       <c r="H453"/>
       <c r="I453" s="1"/>
-      <c r="J453" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="454" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A454">
@@ -14785,9 +14289,6 @@
       </c>
       <c r="H454"/>
       <c r="I454" s="1"/>
-      <c r="J454" s="1">
-        <v>-32.369999999999997</v>
-      </c>
     </row>
     <row r="455" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A455">
@@ -14810,9 +14311,6 @@
       </c>
       <c r="H455"/>
       <c r="I455" s="1"/>
-      <c r="J455" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="456" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A456">
@@ -14835,9 +14333,6 @@
       </c>
       <c r="H456"/>
       <c r="I456" s="1"/>
-      <c r="J456" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="457" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A457">
@@ -14860,9 +14355,6 @@
       </c>
       <c r="H457"/>
       <c r="I457" s="1"/>
-      <c r="J457" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="458" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A458">
@@ -14885,9 +14377,6 @@
       </c>
       <c r="H458"/>
       <c r="I458" s="1"/>
-      <c r="J458" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="459" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A459">
@@ -14910,9 +14399,6 @@
       </c>
       <c r="H459"/>
       <c r="I459" s="1"/>
-      <c r="J459" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="460" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A460">
@@ -14934,9 +14420,11 @@
         <v>18.52</v>
       </c>
       <c r="H460"/>
-      <c r="I460" s="1"/>
+      <c r="I460" s="1">
+        <v>19</v>
+      </c>
       <c r="J460" s="1">
-        <v>-18.52</v>
+        <v>0.48000000000000043</v>
       </c>
     </row>
     <row r="461" spans="1:10" x14ac:dyDescent="0.2">
@@ -14963,9 +14451,6 @@
       </c>
       <c r="H461"/>
       <c r="I461" s="1"/>
-      <c r="J461" s="1">
-        <v>-29.63</v>
-      </c>
     </row>
     <row r="462" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A462">
@@ -14988,9 +14473,6 @@
       </c>
       <c r="H462"/>
       <c r="I462" s="1"/>
-      <c r="J462" s="1">
-        <v>-22.22</v>
-      </c>
     </row>
     <row r="463" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A463">
@@ -15013,9 +14495,6 @@
       </c>
       <c r="H463"/>
       <c r="I463" s="1"/>
-      <c r="J463" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="464" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A464">
@@ -15038,11 +14517,8 @@
       </c>
       <c r="H464"/>
       <c r="I464" s="1"/>
-      <c r="J464" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>1</v>
       </c>
@@ -15063,11 +14539,8 @@
       </c>
       <c r="H465"/>
       <c r="I465" s="1"/>
-      <c r="J465" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>1</v>
       </c>
@@ -15088,11 +14561,8 @@
       </c>
       <c r="H466"/>
       <c r="I466" s="1"/>
-      <c r="J466" s="1">
-        <v>-33.33</v>
-      </c>
-    </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>1</v>
       </c>
@@ -15113,11 +14583,8 @@
       </c>
       <c r="H467"/>
       <c r="I467" s="1"/>
-      <c r="J467" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>1</v>
       </c>
@@ -15138,11 +14605,8 @@
       </c>
       <c r="H468"/>
       <c r="I468" s="1"/>
-      <c r="J468" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="469" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>1</v>
       </c>
@@ -15163,11 +14627,8 @@
       </c>
       <c r="H469"/>
       <c r="I469" s="1"/>
-      <c r="J469" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="470" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>1</v>
       </c>
@@ -15188,11 +14649,8 @@
       </c>
       <c r="H470"/>
       <c r="I470" s="1"/>
-      <c r="J470" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="471" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>1</v>
       </c>
@@ -15213,11 +14671,8 @@
       </c>
       <c r="H471"/>
       <c r="I471" s="1"/>
-      <c r="J471" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="472" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>1</v>
       </c>
@@ -15238,11 +14693,8 @@
       </c>
       <c r="H472"/>
       <c r="I472" s="1"/>
-      <c r="J472" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="473" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>1</v>
       </c>
@@ -15263,11 +14715,8 @@
       </c>
       <c r="H473"/>
       <c r="I473" s="1"/>
-      <c r="J473" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="474" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A474">
         <v>1</v>
       </c>
@@ -15288,11 +14737,8 @@
       </c>
       <c r="H474"/>
       <c r="I474" s="1"/>
-      <c r="J474" s="1">
-        <v>-22.22</v>
-      </c>
-    </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="475" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>1</v>
       </c>
@@ -15313,11 +14759,8 @@
       </c>
       <c r="H475"/>
       <c r="I475" s="1"/>
-      <c r="J475" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="476" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>1</v>
       </c>
@@ -15338,11 +14781,8 @@
       </c>
       <c r="H476"/>
       <c r="I476" s="1"/>
-      <c r="J476" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="477" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>1</v>
       </c>
@@ -15363,11 +14803,8 @@
       </c>
       <c r="H477"/>
       <c r="I477" s="1"/>
-      <c r="J477" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="478" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>1</v>
       </c>
@@ -15388,11 +14825,8 @@
       </c>
       <c r="H478"/>
       <c r="I478" s="1"/>
-      <c r="J478" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="479" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>1</v>
       </c>
@@ -15413,11 +14847,8 @@
       </c>
       <c r="H479"/>
       <c r="I479" s="1"/>
-      <c r="J479" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="480" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>1</v>
       </c>
@@ -15438,9 +14869,6 @@
       </c>
       <c r="H480"/>
       <c r="I480" s="1"/>
-      <c r="J480" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="481" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A481">
@@ -15463,9 +14891,6 @@
       </c>
       <c r="H481"/>
       <c r="I481" s="1"/>
-      <c r="J481" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="482" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A482">
@@ -15488,9 +14913,6 @@
       </c>
       <c r="H482"/>
       <c r="I482" s="1"/>
-      <c r="J482" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="483" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A483">
@@ -15512,9 +14934,11 @@
         <v>17.04</v>
       </c>
       <c r="H483"/>
-      <c r="I483" s="1"/>
+      <c r="I483" s="1">
+        <v>19.8</v>
+      </c>
       <c r="J483" s="1">
-        <v>-17.04</v>
+        <v>2.7600000000000016</v>
       </c>
     </row>
     <row r="484" spans="1:10" x14ac:dyDescent="0.2">
@@ -15538,9 +14962,6 @@
       </c>
       <c r="H484"/>
       <c r="I484" s="1"/>
-      <c r="J484" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="485" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A485">
@@ -15563,9 +14984,6 @@
       </c>
       <c r="H485"/>
       <c r="I485" s="1"/>
-      <c r="J485" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="486" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A486">
@@ -15588,9 +15006,6 @@
       </c>
       <c r="H486"/>
       <c r="I486" s="1"/>
-      <c r="J486" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="487" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A487">
@@ -15613,9 +15028,6 @@
       </c>
       <c r="H487"/>
       <c r="I487" s="1"/>
-      <c r="J487" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="488" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A488">
@@ -15641,9 +15053,6 @@
       </c>
       <c r="H488"/>
       <c r="I488" s="1"/>
-      <c r="J488" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="489" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A489">
@@ -15666,9 +15075,6 @@
       </c>
       <c r="H489"/>
       <c r="I489" s="1"/>
-      <c r="J489" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="490" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A490">
@@ -15691,9 +15097,6 @@
       </c>
       <c r="H490"/>
       <c r="I490" s="1"/>
-      <c r="J490" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="491" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A491">
@@ -15716,9 +15119,6 @@
       </c>
       <c r="H491"/>
       <c r="I491" s="1"/>
-      <c r="J491" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
     <row r="492" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A492">
@@ -15741,9 +15141,6 @@
       </c>
       <c r="H492"/>
       <c r="I492" s="1"/>
-      <c r="J492" s="1">
-        <v>-17.04</v>
-      </c>
     </row>
     <row r="493" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A493">
@@ -15766,9 +15163,6 @@
       </c>
       <c r="H493"/>
       <c r="I493" s="1"/>
-      <c r="J493" s="1">
-        <v>-18.52</v>
-      </c>
     </row>
     <row r="494" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A494">
@@ -15791,9 +15185,6 @@
       </c>
       <c r="H494"/>
       <c r="I494" s="1"/>
-      <c r="J494" s="1">
-        <v>-40.74</v>
-      </c>
     </row>
     <row r="495" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A495">
@@ -15816,9 +15207,6 @@
       </c>
       <c r="H495"/>
       <c r="I495" s="1"/>
-      <c r="J495" s="1">
-        <v>-29.63</v>
-      </c>
     </row>
     <row r="496" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A496">
@@ -15841,11 +15229,8 @@
       </c>
       <c r="H496"/>
       <c r="I496" s="1"/>
-      <c r="J496" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="497" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="497" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A497">
         <v>1</v>
       </c>
@@ -15866,11 +15251,8 @@
       </c>
       <c r="H497"/>
       <c r="I497" s="1"/>
-      <c r="J497" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="498" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="498" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A498">
         <v>1</v>
       </c>
@@ -15891,11 +15273,8 @@
       </c>
       <c r="H498"/>
       <c r="I498" s="1"/>
-      <c r="J498" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="499" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A499">
         <v>1</v>
       </c>
@@ -15916,11 +15295,8 @@
       </c>
       <c r="H499"/>
       <c r="I499" s="1"/>
-      <c r="J499" s="1">
-        <v>-18.52</v>
-      </c>
-    </row>
-    <row r="500" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A500">
         <v>1</v>
       </c>
@@ -15941,11 +15317,8 @@
       </c>
       <c r="H500"/>
       <c r="I500" s="1"/>
-      <c r="J500" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="501" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A501">
         <v>1</v>
       </c>
@@ -15966,11 +15339,8 @@
       </c>
       <c r="H501"/>
       <c r="I501" s="1"/>
-      <c r="J501" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="502" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="502" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A502">
         <v>1</v>
       </c>
@@ -15991,11 +15361,8 @@
       </c>
       <c r="H502"/>
       <c r="I502" s="1"/>
-      <c r="J502" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="503" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="503" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A503">
         <v>1</v>
       </c>
@@ -16016,11 +15383,8 @@
       </c>
       <c r="H503"/>
       <c r="I503" s="1"/>
-      <c r="J503" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="504" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="504" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A504">
         <v>1</v>
       </c>
@@ -16041,11 +15405,8 @@
       </c>
       <c r="H504"/>
       <c r="I504" s="1"/>
-      <c r="J504" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="505" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="505" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A505">
         <v>1</v>
       </c>
@@ -16066,11 +15427,8 @@
       </c>
       <c r="H505"/>
       <c r="I505" s="1"/>
-      <c r="J505" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="506" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="506" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A506">
         <v>1</v>
       </c>
@@ -16091,11 +15449,8 @@
       </c>
       <c r="H506"/>
       <c r="I506" s="1"/>
-      <c r="J506" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="507" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="507" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A507">
         <v>1</v>
       </c>
@@ -16116,11 +15471,8 @@
       </c>
       <c r="H507"/>
       <c r="I507" s="1"/>
-      <c r="J507" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="508" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="508" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A508">
         <v>1</v>
       </c>
@@ -16141,11 +15493,8 @@
       </c>
       <c r="H508"/>
       <c r="I508" s="1"/>
-      <c r="J508" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="509" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="509" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A509">
         <v>1</v>
       </c>
@@ -16166,11 +15515,8 @@
       </c>
       <c r="H509"/>
       <c r="I509" s="1"/>
-      <c r="J509" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="510" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A510">
         <v>1</v>
       </c>
@@ -16191,11 +15537,8 @@
       </c>
       <c r="H510"/>
       <c r="I510" s="1"/>
-      <c r="J510" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="511" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="511" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A511">
         <v>1</v>
       </c>
@@ -16215,11 +15558,8 @@
         <v>17.04</v>
       </c>
       <c r="I511" s="1"/>
-      <c r="J511" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="512" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="512" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A512">
         <v>1</v>
       </c>
@@ -16239,11 +15579,8 @@
         <v>17.04</v>
       </c>
       <c r="I512" s="1"/>
-      <c r="J512" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="513" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="513" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A513">
         <v>1</v>
       </c>
@@ -16263,11 +15600,8 @@
         <v>17.04</v>
       </c>
       <c r="I513" s="1"/>
-      <c r="J513" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="514" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="514" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A514">
         <v>1</v>
       </c>
@@ -16287,11 +15621,8 @@
         <v>17.04</v>
       </c>
       <c r="I514" s="1"/>
-      <c r="J514" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="515" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="515" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A515">
         <v>1</v>
       </c>
@@ -16311,11 +15642,8 @@
         <v>25.93</v>
       </c>
       <c r="I515" s="1"/>
-      <c r="J515" s="1">
-        <v>-25.93</v>
-      </c>
-    </row>
-    <row r="516" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="516" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A516">
         <v>1</v>
       </c>
@@ -16335,11 +15663,8 @@
         <v>17.04</v>
       </c>
       <c r="I516" s="1"/>
-      <c r="J516" s="1">
-        <v>-17.04</v>
-      </c>
-    </row>
-    <row r="517" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="517" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A517">
         <v>1</v>
       </c>
@@ -16359,9 +15684,6 @@
         <v>25.93</v>
       </c>
       <c r="I517" s="1"/>
-      <c r="J517" s="1">
-        <v>-25.93</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J517" xr:uid="{7B1841C9-D21C-2040-9467-2F510B1F6134}"/>

</xml_diff>

<commit_message>
2nd update for round 4 projections
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D726E21-6C8F-014A-A984-3CC746BCA622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AC9DC5-A0D7-4C49-B3FB-D29E7ED1AA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30180" yWindow="3560" windowWidth="25400" windowHeight="16360" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="2240" yWindow="1860" windowWidth="24780" windowHeight="14680" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -1690,7 +1690,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1821,6 +1821,19 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2168,7 +2181,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2177,6 +2190,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2556,10 +2571,10 @@
   <dimension ref="A1:K517"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="M228" sqref="M228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2622,11 +2637,11 @@
         <v>70.3</v>
       </c>
       <c r="H2"/>
-      <c r="I2" s="1">
-        <v>68.2</v>
+      <c r="I2" s="4">
+        <v>74.400000000000006</v>
       </c>
       <c r="J2" s="1">
-        <v>-2.0999999999999943</v>
+        <v>4.1000000000000085</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -6210,11 +6225,11 @@
         <v>28</v>
       </c>
       <c r="H132"/>
-      <c r="I132" s="1">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="J132" s="1">
-        <v>6.7999999999999972</v>
+      <c r="I132" s="4">
+        <v>39.4</v>
+      </c>
+      <c r="J132" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
@@ -8945,12 +8960,7 @@
         <v>36.22</v>
       </c>
       <c r="H233"/>
-      <c r="I233" s="1">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="J233" s="1">
-        <v>-3.9200000000000017</v>
-      </c>
+      <c r="I233" s="1"/>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234">

</xml_diff>

<commit_message>
rnd 5 - 2nd projections update
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB550443-4FD9-0D4B-B0E6-C826484C568F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48299736-5717-8E40-AB8A-797D800C2D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31720" yWindow="1700" windowWidth="24780" windowHeight="14680" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="2120" yWindow="1120" windowWidth="24780" windowHeight="14680" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -2575,10 +2575,10 @@
   <dimension ref="A1:K521"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3559,10 +3559,10 @@
       </c>
       <c r="H35"/>
       <c r="I35" s="4">
-        <v>56.3</v>
+        <v>53.8</v>
       </c>
       <c r="J35" s="1">
-        <v>9.11</v>
+        <v>6.6099999999999994</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -3859,10 +3859,10 @@
       </c>
       <c r="H46"/>
       <c r="I46" s="4">
-        <v>55.7</v>
+        <v>57.8</v>
       </c>
       <c r="J46" s="1">
-        <v>4.1400000000000006</v>
+        <v>6.2399999999999949</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4805,10 +4805,10 @@
       </c>
       <c r="H80"/>
       <c r="I80" s="4">
-        <v>54.5</v>
+        <v>52.1</v>
       </c>
       <c r="J80" s="1">
-        <v>9.1700000000000017</v>
+        <v>6.7700000000000031</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -5469,10 +5469,10 @@
       </c>
       <c r="H104"/>
       <c r="I104" s="4">
-        <v>47.9</v>
+        <v>45.2</v>
       </c>
       <c r="J104" s="1">
-        <v>7.75</v>
+        <v>5.0500000000000043</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
@@ -5826,10 +5826,10 @@
       </c>
       <c r="H117"/>
       <c r="I117" s="4">
-        <v>47.1</v>
+        <v>44.7</v>
       </c>
       <c r="J117" s="1">
-        <v>11.170000000000002</v>
+        <v>8.7700000000000031</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -7363,10 +7363,10 @@
       </c>
       <c r="H173"/>
       <c r="I173" s="4">
-        <v>49</v>
+        <v>44.1</v>
       </c>
       <c r="J173" s="1">
-        <v>8.4799999999999969</v>
+        <v>3.5799999999999983</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
@@ -7582,10 +7582,10 @@
       </c>
       <c r="H181"/>
       <c r="I181" s="4">
-        <v>40</v>
+        <v>38.4</v>
       </c>
       <c r="J181" s="1">
-        <v>11.850000000000001</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
@@ -7905,10 +7905,10 @@
       </c>
       <c r="H193"/>
       <c r="I193" s="4">
-        <v>24.7</v>
+        <v>23.8</v>
       </c>
       <c r="J193" s="1">
-        <v>5</v>
+        <v>4.1000000000000014</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
@@ -8785,10 +8785,10 @@
       </c>
       <c r="H225"/>
       <c r="I225" s="4">
-        <v>35.200000000000003</v>
+        <v>34.1</v>
       </c>
       <c r="J225" s="1">
-        <v>0.16000000000000369</v>
+        <v>-0.93999999999999773</v>
       </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.2">
@@ -9675,9 +9675,11 @@
         <v>36.22</v>
       </c>
       <c r="H258"/>
-      <c r="I258" s="4"/>
+      <c r="I258" s="4">
+        <v>33.299999999999997</v>
+      </c>
       <c r="J258" s="1">
-        <v>-36.22</v>
+        <v>-2.9200000000000017</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.2">
@@ -10193,10 +10195,10 @@
       </c>
       <c r="H277"/>
       <c r="I277" s="4">
-        <v>31.6</v>
+        <v>32.4</v>
       </c>
       <c r="J277" s="1">
-        <v>6.120000000000001</v>
+        <v>6.9199999999999982</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.2">
@@ -10439,10 +10441,10 @@
       </c>
       <c r="H286"/>
       <c r="I286" s="4">
-        <v>21</v>
+        <v>31.9</v>
       </c>
       <c r="J286" s="1">
-        <v>3.9999999999999147E-2</v>
+        <v>10.939999999999998</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.2">
@@ -11641,9 +11643,11 @@
         <v>17.04</v>
       </c>
       <c r="H331"/>
-      <c r="I331" s="4"/>
+      <c r="I331" s="4">
+        <v>11.8</v>
+      </c>
       <c r="J331" s="1">
-        <v>-17.04</v>
+        <v>-5.2399999999999984</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update prices for round 6 (post TLT projection updates)
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E688EF2-E6D5-CD4E-B92A-A5DA56F75EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B849A7F-8FB4-714E-9077-31F4B0A11F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="1260" windowWidth="23800" windowHeight="14500" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="3860" yWindow="2040" windowWidth="23800" windowHeight="14500" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -2584,10 +2584,10 @@
   <dimension ref="A1:K524"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C346" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="J359" sqref="J359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2755,7 +2755,7 @@
         <v>57.8</v>
       </c>
       <c r="J6" s="1">
-        <f>I6-G6</f>
+        <f t="shared" ref="J6:J37" si="0">I6-G6</f>
         <v>3.6499999999999986</v>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="J7" s="1">
-        <f>I7-G7</f>
+        <f t="shared" si="0"/>
         <v>-7.9699999999999989</v>
       </c>
     </row>
@@ -2814,7 +2814,7 @@
         <v>52.3</v>
       </c>
       <c r="J8" s="1">
-        <f>I8-G8</f>
+        <f t="shared" si="0"/>
         <v>0.6699999999999946</v>
       </c>
     </row>
@@ -2842,7 +2842,7 @@
         <v>46.9</v>
       </c>
       <c r="J9" s="1">
-        <f>I9-G9</f>
+        <f t="shared" si="0"/>
         <v>0.22999999999999687</v>
       </c>
     </row>
@@ -2870,7 +2870,7 @@
         <v>50.6</v>
       </c>
       <c r="J10" s="1">
-        <f>I10-G10</f>
+        <f t="shared" si="0"/>
         <v>-5.0300000000000011</v>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
         <v>62.1</v>
       </c>
       <c r="J11" s="1">
-        <f>I11-G11</f>
+        <f t="shared" si="0"/>
         <v>5.8800000000000026</v>
       </c>
     </row>
@@ -2932,7 +2932,7 @@
         <v>55.6</v>
       </c>
       <c r="J12" s="1">
-        <f>I12-G12</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000014</v>
       </c>
     </row>
@@ -2960,7 +2960,7 @@
         <v>63</v>
       </c>
       <c r="J13" s="1">
-        <f>I13-G13</f>
+        <f t="shared" si="0"/>
         <v>4.6300000000000026</v>
       </c>
     </row>
@@ -2988,7 +2988,7 @@
         <v>51.4</v>
       </c>
       <c r="J14" s="1">
-        <f>I14-G14</f>
+        <f t="shared" si="0"/>
         <v>-4.8999999999999986</v>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
         <v>46.5</v>
       </c>
       <c r="J15" s="1">
-        <f>I15-G15</f>
+        <f t="shared" si="0"/>
         <v>-3.1300000000000026</v>
       </c>
     </row>
@@ -3044,7 +3044,7 @@
         <v>58.5</v>
       </c>
       <c r="J16" s="1">
-        <f>I16-G16</f>
+        <f t="shared" si="0"/>
         <v>4.2800000000000011</v>
       </c>
     </row>
@@ -3072,7 +3072,7 @@
         <v>45.7</v>
       </c>
       <c r="J17" s="1">
-        <f>I17-G17</f>
+        <f t="shared" si="0"/>
         <v>-0.36999999999999744</v>
       </c>
     </row>
@@ -3103,7 +3103,7 @@
         <v>51.6</v>
       </c>
       <c r="J18" s="1">
-        <f>I18-G18</f>
+        <f t="shared" si="0"/>
         <v>-2.3299999999999983</v>
       </c>
     </row>
@@ -3128,11 +3128,11 @@
       </c>
       <c r="H19"/>
       <c r="I19" s="4">
-        <v>52.3</v>
+        <v>49.4</v>
       </c>
       <c r="J19" s="1">
-        <f>I19-G19</f>
-        <v>-1.7700000000000031</v>
+        <f t="shared" si="0"/>
+        <v>-4.6700000000000017</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -3159,7 +3159,7 @@
         <v>51.5</v>
       </c>
       <c r="J20" s="1">
-        <f>I20-G20</f>
+        <f t="shared" si="0"/>
         <v>-4.0600000000000023</v>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
         <v>46.9</v>
       </c>
       <c r="J21" s="1">
-        <f>I21-G21</f>
+        <f t="shared" si="0"/>
         <v>3.269999999999996</v>
       </c>
     </row>
@@ -3215,7 +3215,7 @@
         <v>51.4</v>
       </c>
       <c r="J22" s="1">
-        <f>I22-G22</f>
+        <f t="shared" si="0"/>
         <v>-1.7899999999999991</v>
       </c>
     </row>
@@ -3243,7 +3243,7 @@
         <v>36</v>
       </c>
       <c r="J23" s="1">
-        <f>I23-G23</f>
+        <f t="shared" si="0"/>
         <v>-12.740000000000002</v>
       </c>
     </row>
@@ -3271,7 +3271,7 @@
         <v>52</v>
       </c>
       <c r="J24" s="1">
-        <f>I24-G24</f>
+        <f t="shared" si="0"/>
         <v>-0.96000000000000085</v>
       </c>
     </row>
@@ -3299,7 +3299,7 @@
         <v>43.5</v>
       </c>
       <c r="J25" s="1">
-        <f>I25-G25</f>
+        <f t="shared" si="0"/>
         <v>-7.4600000000000009</v>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
         <v>39.299999999999997</v>
       </c>
       <c r="J26" s="1">
-        <f>I26-G26</f>
+        <f t="shared" si="0"/>
         <v>-2.1099999999999994</v>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
         <v>56.9</v>
       </c>
       <c r="J27" s="1">
-        <f>I27-G27</f>
+        <f t="shared" si="0"/>
         <v>3.4200000000000017</v>
       </c>
     </row>
@@ -3386,7 +3386,7 @@
         <v>48.2</v>
       </c>
       <c r="J28" s="1">
-        <f>I28-G28</f>
+        <f t="shared" si="0"/>
         <v>-0.46999999999999886</v>
       </c>
     </row>
@@ -3414,7 +3414,7 @@
         <v>52.9</v>
       </c>
       <c r="J29" s="1">
-        <f>I29-G29</f>
+        <f t="shared" si="0"/>
         <v>5.9399999999999977</v>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
         <v>41.8</v>
       </c>
       <c r="J30" s="1">
-        <f>I30-G30</f>
+        <f t="shared" si="0"/>
         <v>-4.0500000000000043</v>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
         <v>42.7</v>
       </c>
       <c r="J31" s="1">
-        <f>I31-G31</f>
+        <f t="shared" si="0"/>
         <v>-6.6299999999999955</v>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
         <v>44.5</v>
       </c>
       <c r="J32" s="1">
-        <f>I32-G32</f>
+        <f t="shared" si="0"/>
         <v>-9.0000000000003411E-2</v>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
         <v>46.6</v>
       </c>
       <c r="J33" s="1">
-        <f>I33-G33</f>
+        <f t="shared" si="0"/>
         <v>-2.4399999999999977</v>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
         <v>42.7</v>
       </c>
       <c r="J34" s="1">
-        <f>I34-G34</f>
+        <f t="shared" si="0"/>
         <v>-4.1899999999999977</v>
       </c>
     </row>
@@ -3585,7 +3585,7 @@
         <v>55.1</v>
       </c>
       <c r="J35" s="1">
-        <f>I35-G35</f>
+        <f t="shared" si="0"/>
         <v>3.0300000000000011</v>
       </c>
     </row>
@@ -3613,7 +3613,7 @@
         <v>59.9</v>
       </c>
       <c r="J36" s="1">
-        <f>I36-G36</f>
+        <f t="shared" si="0"/>
         <v>8.1999999999999957</v>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
         <v>51.8</v>
       </c>
       <c r="J37" s="1">
-        <f>I37-G37</f>
+        <f t="shared" si="0"/>
         <v>3.5799999999999983</v>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
         <v>55.5</v>
       </c>
       <c r="J38" s="1">
-        <f>I38-G38</f>
+        <f t="shared" ref="J38:J63" si="1">I38-G38</f>
         <v>-0.79999999999999716</v>
       </c>
     </row>
@@ -3697,7 +3697,7 @@
         <v>42.8</v>
       </c>
       <c r="J39" s="1">
-        <f>I39-G39</f>
+        <f t="shared" si="1"/>
         <v>-7.9400000000000048</v>
       </c>
     </row>
@@ -3728,7 +3728,7 @@
         <v>49.4</v>
       </c>
       <c r="J40" s="1">
-        <f>I40-G40</f>
+        <f t="shared" si="1"/>
         <v>-0.60000000000000142</v>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
         <v>46.8</v>
       </c>
       <c r="J41" s="1">
-        <f>I41-G41</f>
+        <f t="shared" si="1"/>
         <v>-3.7900000000000063</v>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
         <v>47.3</v>
       </c>
       <c r="J42" s="1">
-        <f>I42-G42</f>
+        <f t="shared" si="1"/>
         <v>-2.1099999999999994</v>
       </c>
     </row>
@@ -3818,7 +3818,7 @@
         <v>31.3</v>
       </c>
       <c r="J43" s="1">
-        <f>I43-G43</f>
+        <f t="shared" si="1"/>
         <v>-16.330000000000002</v>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
         <v>52.8</v>
       </c>
       <c r="J44" s="1">
-        <f>I44-G44</f>
+        <f t="shared" si="1"/>
         <v>0.20999999999999375</v>
       </c>
     </row>
@@ -3874,7 +3874,7 @@
         <v>50.6</v>
       </c>
       <c r="J45" s="1">
-        <f>I45-G45</f>
+        <f t="shared" si="1"/>
         <v>-0.72999999999999687</v>
       </c>
     </row>
@@ -3902,7 +3902,7 @@
         <v>51.2</v>
       </c>
       <c r="J46" s="1">
-        <f>I46-G46</f>
+        <f t="shared" si="1"/>
         <v>3.6400000000000006</v>
       </c>
     </row>
@@ -3930,11 +3930,11 @@
       </c>
       <c r="H47"/>
       <c r="I47" s="4">
-        <v>50.1</v>
+        <v>42.5</v>
       </c>
       <c r="J47" s="1">
-        <f>I47-G47</f>
-        <v>-2.490000000000002</v>
+        <f t="shared" si="1"/>
+        <v>-10.090000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -3961,7 +3961,7 @@
         <v>50.6</v>
       </c>
       <c r="J48" s="1">
-        <f>I48-G48</f>
+        <f t="shared" si="1"/>
         <v>1.1200000000000045</v>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
         <v>44.5</v>
       </c>
       <c r="J49" s="1">
-        <f>I49-G49</f>
+        <f t="shared" si="1"/>
         <v>-0.53999999999999915</v>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
         <v>54.5</v>
       </c>
       <c r="J50" s="1">
-        <f>I50-G50</f>
+        <f t="shared" si="1"/>
         <v>4.2800000000000011</v>
       </c>
     </row>
@@ -4048,7 +4048,7 @@
         <v>48.2</v>
       </c>
       <c r="J51" s="1">
-        <f>I51-G51</f>
+        <f t="shared" si="1"/>
         <v>-1.1299999999999955</v>
       </c>
     </row>
@@ -4079,7 +4079,7 @@
         <v>50.7</v>
       </c>
       <c r="J52" s="1">
-        <f>I52-G52</f>
+        <f t="shared" si="1"/>
         <v>-0.18999999999999773</v>
       </c>
     </row>
@@ -4107,7 +4107,7 @@
         <v>50.3</v>
       </c>
       <c r="J53" s="1">
-        <f>I53-G53</f>
+        <f t="shared" si="1"/>
         <v>2.3699999999999974</v>
       </c>
     </row>
@@ -4135,7 +4135,7 @@
         <v>58.6</v>
       </c>
       <c r="J54" s="1">
-        <f>I54-G54</f>
+        <f t="shared" si="1"/>
         <v>5.5600000000000023</v>
       </c>
     </row>
@@ -4163,7 +4163,7 @@
         <v>48.2</v>
       </c>
       <c r="J55" s="1">
-        <f>I55-G55</f>
+        <f t="shared" si="1"/>
         <v>-0.60999999999999943</v>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
         <v>71.2</v>
       </c>
       <c r="J56" s="1">
-        <f>I56-G56</f>
+        <f t="shared" si="1"/>
         <v>16.010000000000005</v>
       </c>
     </row>
@@ -4219,7 +4219,7 @@
         <v>43.5</v>
       </c>
       <c r="J57" s="1">
-        <f>I57-G57</f>
+        <f t="shared" si="1"/>
         <v>-2.2800000000000011</v>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
         <v>42.1</v>
       </c>
       <c r="J58" s="1">
-        <f>I58-G58</f>
+        <f t="shared" si="1"/>
         <v>-5.5300000000000011</v>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
         <v>48.5</v>
       </c>
       <c r="J59" s="1">
-        <f>I59-G59</f>
+        <f t="shared" si="1"/>
         <v>1.3900000000000006</v>
       </c>
     </row>
@@ -4303,7 +4303,7 @@
         <v>51.4</v>
       </c>
       <c r="J60" s="1">
-        <f>I60-G60</f>
+        <f t="shared" si="1"/>
         <v>5.6999999999999957</v>
       </c>
     </row>
@@ -4331,7 +4331,7 @@
         <v>46.5</v>
       </c>
       <c r="J61" s="1">
-        <f>I61-G61</f>
+        <f t="shared" si="1"/>
         <v>3.4600000000000009</v>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
         <v>46</v>
       </c>
       <c r="J62" s="1">
-        <f>I62-G62</f>
+        <f t="shared" si="1"/>
         <v>-1.7000000000000028</v>
       </c>
     </row>
@@ -4390,7 +4390,7 @@
         <v>50.7</v>
       </c>
       <c r="J63" s="1">
-        <f>I63-G63</f>
+        <f t="shared" si="1"/>
         <v>5.9600000000000009</v>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
         <v>33.299999999999997</v>
       </c>
       <c r="J65" s="1">
-        <f>I65-G65</f>
+        <f t="shared" ref="J65:J99" si="2">I65-G65</f>
         <v>-12.260000000000005</v>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
         <v>45.5</v>
       </c>
       <c r="J66" s="1">
-        <f>I66-G66</f>
+        <f t="shared" si="2"/>
         <v>0.31000000000000227</v>
       </c>
     </row>
@@ -4502,7 +4502,7 @@
         <v>31.6</v>
       </c>
       <c r="J67" s="1">
-        <f>I67-G67</f>
+        <f t="shared" si="2"/>
         <v>-8.6199999999999974</v>
       </c>
     </row>
@@ -4530,7 +4530,7 @@
         <v>34</v>
       </c>
       <c r="J68" s="1">
-        <f>I68-G68</f>
+        <f t="shared" si="2"/>
         <v>1.1899999999999977</v>
       </c>
     </row>
@@ -4558,7 +4558,7 @@
         <v>52.9</v>
       </c>
       <c r="J69" s="1">
-        <f>I69-G69</f>
+        <f t="shared" si="2"/>
         <v>5.57</v>
       </c>
     </row>
@@ -4586,7 +4586,7 @@
         <v>39.200000000000003</v>
       </c>
       <c r="J70" s="1">
-        <f>I70-G70</f>
+        <f t="shared" si="2"/>
         <v>-2.7299999999999969</v>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
         <v>57.4</v>
       </c>
       <c r="J71" s="1">
-        <f>I71-G71</f>
+        <f t="shared" si="2"/>
         <v>-0.67000000000000171</v>
       </c>
     </row>
@@ -4642,7 +4642,7 @@
         <v>45.2</v>
       </c>
       <c r="J72" s="1">
-        <f>I72-G72</f>
+        <f t="shared" si="2"/>
         <v>2.3900000000000006</v>
       </c>
     </row>
@@ -4673,7 +4673,7 @@
         <v>42.6</v>
       </c>
       <c r="J73" s="1">
-        <f>I73-G73</f>
+        <f t="shared" si="2"/>
         <v>2.6000000000000014</v>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
         <v>35.6</v>
       </c>
       <c r="J74" s="1">
-        <f>I74-G74</f>
+        <f t="shared" si="2"/>
         <v>3.9999999999999147E-2</v>
       </c>
     </row>
@@ -4732,7 +4732,7 @@
         <v>42</v>
       </c>
       <c r="J75" s="1">
-        <f>I75-G75</f>
+        <f t="shared" si="2"/>
         <v>-0.96000000000000085</v>
       </c>
     </row>
@@ -4760,7 +4760,7 @@
         <v>40.9</v>
       </c>
       <c r="J76" s="1">
-        <f>I76-G76</f>
+        <f t="shared" si="2"/>
         <v>-2.4299999999999997</v>
       </c>
     </row>
@@ -4791,7 +4791,7 @@
         <v>39.5</v>
       </c>
       <c r="J77" s="1">
-        <f>I77-G77</f>
+        <f t="shared" si="2"/>
         <v>-3.4600000000000009</v>
       </c>
     </row>
@@ -4819,7 +4819,7 @@
         <v>52.1</v>
       </c>
       <c r="J78" s="1">
-        <f>I78-G78</f>
+        <f t="shared" si="2"/>
         <v>6.3999999999999986</v>
       </c>
     </row>
@@ -4850,7 +4850,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="J79" s="1">
-        <f>I79-G79</f>
+        <f t="shared" si="2"/>
         <v>-5.18</v>
       </c>
     </row>
@@ -4878,7 +4878,7 @@
         <v>43.5</v>
       </c>
       <c r="J80" s="1">
-        <f>I80-G80</f>
+        <f t="shared" si="2"/>
         <v>2.0900000000000034</v>
       </c>
     </row>
@@ -4909,7 +4909,7 @@
         <v>48.4</v>
       </c>
       <c r="J81" s="1">
-        <f>I81-G81</f>
+        <f t="shared" si="2"/>
         <v>6.5499999999999972</v>
       </c>
     </row>
@@ -4937,7 +4937,7 @@
         <v>40.5</v>
       </c>
       <c r="J82" s="1">
-        <f>I82-G82</f>
+        <f t="shared" si="2"/>
         <v>17.39</v>
       </c>
     </row>
@@ -4965,7 +4965,7 @@
         <v>41.9</v>
       </c>
       <c r="J83" s="1">
-        <f>I83-G83</f>
+        <f t="shared" si="2"/>
         <v>-0.84000000000000341</v>
       </c>
     </row>
@@ -4993,7 +4993,7 @@
         <v>48.8</v>
       </c>
       <c r="J84" s="1">
-        <f>I84-G84</f>
+        <f t="shared" si="2"/>
         <v>4.3599999999999994</v>
       </c>
     </row>
@@ -5021,7 +5021,7 @@
         <v>42.3</v>
       </c>
       <c r="J85" s="1">
-        <f>I85-G85</f>
+        <f t="shared" si="2"/>
         <v>4.6699999999999946</v>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
         <v>44.2</v>
       </c>
       <c r="J86" s="1">
-        <f>I86-G86</f>
+        <f t="shared" si="2"/>
         <v>1.0900000000000034</v>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
         <v>47.4</v>
       </c>
       <c r="J87" s="1">
-        <f>I87-G87</f>
+        <f t="shared" si="2"/>
         <v>2.8099999999999952</v>
       </c>
     </row>
@@ -5105,7 +5105,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="J88" s="1">
-        <f>I88-G88</f>
+        <f t="shared" si="2"/>
         <v>-4.9600000000000009</v>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
         <v>46.6</v>
       </c>
       <c r="J89" s="1">
-        <f>I89-G89</f>
+        <f t="shared" si="2"/>
         <v>3.6400000000000006</v>
       </c>
     </row>
@@ -5161,7 +5161,7 @@
         <v>52.6</v>
       </c>
       <c r="J90" s="1">
-        <f>I90-G90</f>
+        <f t="shared" si="2"/>
         <v>4.5300000000000011</v>
       </c>
     </row>
@@ -5192,7 +5192,7 @@
         <v>48.2</v>
       </c>
       <c r="J91" s="1">
-        <f>I91-G91</f>
+        <f t="shared" si="2"/>
         <v>1.1600000000000037</v>
       </c>
     </row>
@@ -5220,7 +5220,7 @@
         <v>30.4</v>
       </c>
       <c r="J92" s="1">
-        <f>I92-G92</f>
+        <f t="shared" si="2"/>
         <v>-13.230000000000004</v>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
         <v>53.1</v>
       </c>
       <c r="J93" s="1">
-        <f>I93-G93</f>
+        <f t="shared" si="2"/>
         <v>6.0600000000000023</v>
       </c>
     </row>
@@ -5279,7 +5279,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J94" s="1">
-        <f>I94-G94</f>
+        <f t="shared" si="2"/>
         <v>-0.66000000000000369</v>
       </c>
     </row>
@@ -5310,7 +5310,7 @@
         <v>50.7</v>
       </c>
       <c r="J95" s="1">
-        <f>I95-G95</f>
+        <f t="shared" si="2"/>
         <v>10.330000000000005</v>
       </c>
     </row>
@@ -5338,7 +5338,7 @@
         <v>43.3</v>
       </c>
       <c r="J96" s="1">
-        <f>I96-G96</f>
+        <f t="shared" si="2"/>
         <v>-5.5900000000000034</v>
       </c>
     </row>
@@ -5369,7 +5369,7 @@
         <v>33.6</v>
       </c>
       <c r="J97" s="1">
-        <f>I97-G97</f>
+        <f t="shared" si="2"/>
         <v>-4.3299999999999983</v>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
         <v>41.2</v>
       </c>
       <c r="J98" s="1">
-        <f>I98-G98</f>
+        <f t="shared" si="2"/>
         <v>1.0000000000005116E-2</v>
       </c>
     </row>
@@ -5425,7 +5425,7 @@
         <v>37.6</v>
       </c>
       <c r="J99" s="1">
-        <f>I99-G99</f>
+        <f t="shared" si="2"/>
         <v>10.64</v>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
         <v>43.5</v>
       </c>
       <c r="J104" s="1">
-        <f>I104-G104</f>
+        <f t="shared" ref="J104:J122" si="3">I104-G104</f>
         <v>3.0600000000000023</v>
       </c>
     </row>
@@ -5581,7 +5581,7 @@
         <v>37.1</v>
       </c>
       <c r="J105" s="1">
-        <f>I105-G105</f>
+        <f t="shared" si="3"/>
         <v>5.620000000000001</v>
       </c>
     </row>
@@ -5609,7 +5609,7 @@
         <v>42.1</v>
       </c>
       <c r="J106" s="1">
-        <f>I106-G106</f>
+        <f t="shared" si="3"/>
         <v>1.6600000000000037</v>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
         <v>36</v>
       </c>
       <c r="J107" s="1">
-        <f>I107-G107</f>
+        <f t="shared" si="3"/>
         <v>1.7800000000000011</v>
       </c>
     </row>
@@ -5665,7 +5665,7 @@
         <v>41.9</v>
       </c>
       <c r="J108" s="1">
-        <f>I108-G108</f>
+        <f t="shared" si="3"/>
         <v>0.42000000000000171</v>
       </c>
     </row>
@@ -5693,7 +5693,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="J109" s="1">
-        <f>I109-G109</f>
+        <f t="shared" si="3"/>
         <v>0.40000000000000568</v>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
         <v>33.299999999999997</v>
       </c>
       <c r="J110" s="1">
-        <f>I110-G110</f>
+        <f t="shared" si="3"/>
         <v>-3.220000000000006</v>
       </c>
     </row>
@@ -5749,7 +5749,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J111" s="1">
-        <f>I111-G111</f>
+        <f t="shared" si="3"/>
         <v>1.4099999999999966</v>
       </c>
     </row>
@@ -5777,7 +5777,7 @@
         <v>35.9</v>
       </c>
       <c r="J112" s="1">
-        <f>I112-G112</f>
+        <f t="shared" si="3"/>
         <v>-6.25</v>
       </c>
     </row>
@@ -5808,7 +5808,7 @@
         <v>44.6</v>
       </c>
       <c r="J113" s="1">
-        <f>I113-G113</f>
+        <f t="shared" si="3"/>
         <v>7.490000000000002</v>
       </c>
     </row>
@@ -5836,7 +5836,7 @@
         <v>48.2</v>
       </c>
       <c r="J114" s="1">
-        <f>I114-G114</f>
+        <f t="shared" si="3"/>
         <v>3.240000000000002</v>
       </c>
     </row>
@@ -5867,7 +5867,7 @@
         <v>42.6</v>
       </c>
       <c r="J115" s="1">
-        <f>I115-G115</f>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
     </row>
@@ -5895,7 +5895,7 @@
         <v>42.3</v>
       </c>
       <c r="J116" s="1">
-        <f>I116-G116</f>
+        <f t="shared" si="3"/>
         <v>6.3699999999999974</v>
       </c>
     </row>
@@ -5926,7 +5926,7 @@
         <v>27.7</v>
       </c>
       <c r="J117" s="1">
-        <f>I117-G117</f>
+        <f t="shared" si="3"/>
         <v>-7.860000000000003</v>
       </c>
     </row>
@@ -5954,7 +5954,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="J118" s="1">
-        <f>I118-G118</f>
+        <f t="shared" si="3"/>
         <v>-2.4899999999999949</v>
       </c>
     </row>
@@ -5985,7 +5985,7 @@
         <v>39.4</v>
       </c>
       <c r="J119" s="1">
-        <f>I119-G119</f>
+        <f t="shared" si="3"/>
         <v>6.07</v>
       </c>
     </row>
@@ -6013,7 +6013,7 @@
         <v>52.9</v>
       </c>
       <c r="J120" s="1">
-        <f>I120-G120</f>
+        <f t="shared" si="3"/>
         <v>0.22999999999999687</v>
       </c>
     </row>
@@ -6041,7 +6041,7 @@
         <v>51.4</v>
       </c>
       <c r="J121" s="1">
-        <f>I121-G121</f>
+        <f t="shared" si="3"/>
         <v>0.50999999999999801</v>
       </c>
     </row>
@@ -6069,7 +6069,7 @@
         <v>50.8</v>
       </c>
       <c r="J122" s="1">
-        <f>I122-G122</f>
+        <f t="shared" si="3"/>
         <v>8.0599999999999952</v>
       </c>
     </row>
@@ -6122,7 +6122,7 @@
         <v>42.9</v>
       </c>
       <c r="J124" s="1">
-        <f>I124-G124</f>
+        <f t="shared" ref="J124:J130" si="4">I124-G124</f>
         <v>2.8999999999999986</v>
       </c>
     </row>
@@ -6150,7 +6150,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="J125" s="1">
-        <f>I125-G125</f>
+        <f t="shared" si="4"/>
         <v>-6.4400000000000048</v>
       </c>
       <c r="K125"/>
@@ -6182,7 +6182,7 @@
         <v>43.5</v>
       </c>
       <c r="J126" s="1">
-        <f>I126-G126</f>
+        <f t="shared" si="4"/>
         <v>10.909999999999997</v>
       </c>
     </row>
@@ -6210,7 +6210,7 @@
         <v>41.1</v>
       </c>
       <c r="J127" s="1">
-        <f>I127-G127</f>
+        <f t="shared" si="4"/>
         <v>15.400000000000002</v>
       </c>
     </row>
@@ -6238,7 +6238,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J128" s="1">
-        <f>I128-G128</f>
+        <f t="shared" si="4"/>
         <v>1.8599999999999994</v>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="J129" s="1">
-        <f>I129-G129</f>
+        <f t="shared" si="4"/>
         <v>2.4699999999999989</v>
       </c>
     </row>
@@ -6297,7 +6297,7 @@
         <v>43.4</v>
       </c>
       <c r="J130" s="1">
-        <f>I130-G130</f>
+        <f t="shared" si="4"/>
         <v>6.4399999999999977</v>
       </c>
     </row>
@@ -6350,7 +6350,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="J132" s="1">
-        <f>I132-G132</f>
+        <f t="shared" ref="J132:J144" si="5">I132-G132</f>
         <v>-8.720000000000006</v>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="J133" s="1">
-        <f>I133-G133</f>
+        <f t="shared" si="5"/>
         <v>-12.79</v>
       </c>
     </row>
@@ -6406,7 +6406,7 @@
         <v>20</v>
       </c>
       <c r="J134" s="1">
-        <f>I134-G134</f>
+        <f t="shared" si="5"/>
         <v>-24.810000000000002</v>
       </c>
     </row>
@@ -6434,7 +6434,7 @@
         <v>36</v>
       </c>
       <c r="J135" s="1">
-        <f>I135-G135</f>
+        <f t="shared" si="5"/>
         <v>-6.07</v>
       </c>
     </row>
@@ -6462,7 +6462,7 @@
         <v>42.6</v>
       </c>
       <c r="J136" s="1">
-        <f>I136-G136</f>
+        <f t="shared" si="5"/>
         <v>1.7899999999999991</v>
       </c>
     </row>
@@ -6490,7 +6490,7 @@
         <v>5.3</v>
       </c>
       <c r="J137" s="1">
-        <f>I137-G137</f>
+        <f t="shared" si="5"/>
         <v>-28.109999999999996</v>
       </c>
     </row>
@@ -6518,7 +6518,7 @@
         <v>48.8</v>
       </c>
       <c r="J138" s="1">
-        <f>I138-G138</f>
+        <f t="shared" si="5"/>
         <v>7.3900000000000006</v>
       </c>
     </row>
@@ -6546,7 +6546,7 @@
         <v>41</v>
       </c>
       <c r="J139" s="1">
-        <f>I139-G139</f>
+        <f t="shared" si="5"/>
         <v>4.4799999999999969</v>
       </c>
     </row>
@@ -6574,7 +6574,7 @@
         <v>43.5</v>
       </c>
       <c r="J140" s="1">
-        <f>I140-G140</f>
+        <f t="shared" si="5"/>
         <v>6.6099999999999994</v>
       </c>
     </row>
@@ -6602,7 +6602,7 @@
         <v>29.6</v>
       </c>
       <c r="J141" s="1">
-        <f>I141-G141</f>
+        <f t="shared" si="5"/>
         <v>-5.2899999999999991</v>
       </c>
     </row>
@@ -6630,7 +6630,7 @@
         <v>37.1</v>
       </c>
       <c r="J142" s="1">
-        <f>I142-G142</f>
+        <f t="shared" si="5"/>
         <v>4.43</v>
       </c>
     </row>
@@ -6658,7 +6658,7 @@
         <v>35.6</v>
       </c>
       <c r="J143" s="1">
-        <f>I143-G143</f>
+        <f t="shared" si="5"/>
         <v>-2.990000000000002</v>
       </c>
     </row>
@@ -6689,7 +6689,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="J144" s="1">
-        <f>I144-G144</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6931,7 +6931,13 @@
         <v>33.630000000000003</v>
       </c>
       <c r="H153"/>
-      <c r="I153" s="4"/>
+      <c r="I153" s="4">
+        <v>37.9</v>
+      </c>
+      <c r="J153" s="1">
+        <f>I153-G153</f>
+        <v>4.269999999999996</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
@@ -6982,11 +6988,11 @@
       </c>
       <c r="H155"/>
       <c r="I155" s="4">
-        <v>38.4</v>
+        <v>32.4</v>
       </c>
       <c r="J155" s="1">
         <f>I155-G155</f>
-        <v>8.3999999999999986</v>
+        <v>2.3999999999999986</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
@@ -7035,7 +7041,7 @@
         <v>27.3</v>
       </c>
       <c r="J157" s="1">
-        <f>I157-G157</f>
+        <f t="shared" ref="J157:J183" si="6">I157-G157</f>
         <v>-8.5500000000000007</v>
       </c>
     </row>
@@ -7066,7 +7072,7 @@
         <v>35</v>
       </c>
       <c r="J158" s="1">
-        <f>I158-G158</f>
+        <f t="shared" si="6"/>
         <v>0.56000000000000227</v>
       </c>
     </row>
@@ -7097,7 +7103,7 @@
         <v>37.9</v>
       </c>
       <c r="J159" s="1">
-        <f>I159-G159</f>
+        <f t="shared" si="6"/>
         <v>6.9399999999999977</v>
       </c>
       <c r="K159"/>
@@ -7129,7 +7135,7 @@
         <v>38.200000000000003</v>
       </c>
       <c r="J160" s="1">
-        <f>I160-G160</f>
+        <f t="shared" si="6"/>
         <v>10.940000000000001</v>
       </c>
     </row>
@@ -7157,7 +7163,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="J161" s="1">
-        <f>I161-G161</f>
+        <f t="shared" si="6"/>
         <v>-3.5500000000000043</v>
       </c>
     </row>
@@ -7188,7 +7194,7 @@
         <v>21.6</v>
       </c>
       <c r="J162" s="1">
-        <f>I162-G162</f>
+        <f t="shared" si="6"/>
         <v>-14.100000000000001</v>
       </c>
     </row>
@@ -7219,7 +7225,7 @@
         <v>39.799999999999997</v>
       </c>
       <c r="J163" s="1">
-        <f>I163-G163</f>
+        <f t="shared" si="6"/>
         <v>1.2099999999999937</v>
       </c>
     </row>
@@ -7250,7 +7256,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J164" s="1">
-        <f>I164-G164</f>
+        <f t="shared" si="6"/>
         <v>5.3399999999999963</v>
       </c>
     </row>
@@ -7278,7 +7284,7 @@
         <v>42.8</v>
       </c>
       <c r="J165" s="1">
-        <f>I165-G165</f>
+        <f t="shared" si="6"/>
         <v>4.279999999999994</v>
       </c>
     </row>
@@ -7306,7 +7312,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="J166" s="1">
-        <f>I166-G166</f>
+        <f t="shared" si="6"/>
         <v>-1.1799999999999997</v>
       </c>
     </row>
@@ -7334,7 +7340,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="J167" s="1">
-        <f>I167-G167</f>
+        <f t="shared" si="6"/>
         <v>4.7600000000000016</v>
       </c>
     </row>
@@ -7365,7 +7371,7 @@
         <v>39.5</v>
       </c>
       <c r="J168" s="1">
-        <f>I168-G168</f>
+        <f t="shared" si="6"/>
         <v>3.0600000000000023</v>
       </c>
     </row>
@@ -7393,7 +7399,7 @@
         <v>42.8</v>
       </c>
       <c r="J169" s="1">
-        <f>I169-G169</f>
+        <f t="shared" si="6"/>
         <v>4.7299999999999969</v>
       </c>
     </row>
@@ -7421,7 +7427,7 @@
         <v>41.3</v>
       </c>
       <c r="J170" s="1">
-        <f>I170-G170</f>
+        <f t="shared" si="6"/>
         <v>3.5999999999999943</v>
       </c>
     </row>
@@ -7449,7 +7455,7 @@
         <v>28.8</v>
       </c>
       <c r="J171" s="1">
-        <f>I171-G171</f>
+        <f t="shared" si="6"/>
         <v>1.990000000000002</v>
       </c>
     </row>
@@ -7477,7 +7483,7 @@
         <v>41.9</v>
       </c>
       <c r="J172" s="1">
-        <f>I172-G172</f>
+        <f t="shared" si="6"/>
         <v>4.269999999999996</v>
       </c>
     </row>
@@ -7505,7 +7511,7 @@
         <v>39.1</v>
       </c>
       <c r="J173" s="1">
-        <f>I173-G173</f>
+        <f t="shared" si="6"/>
         <v>4.43</v>
       </c>
     </row>
@@ -7533,7 +7539,7 @@
         <v>30.8</v>
       </c>
       <c r="J174" s="1">
-        <f>I174-G174</f>
+        <f t="shared" si="6"/>
         <v>-1.129999999999999</v>
       </c>
     </row>
@@ -7561,7 +7567,7 @@
         <v>15</v>
       </c>
       <c r="J175" s="1">
-        <f>I175-G175</f>
+        <f t="shared" si="6"/>
         <v>-15.739999999999998</v>
       </c>
     </row>
@@ -7592,7 +7598,7 @@
         <v>30.8</v>
       </c>
       <c r="J176" s="1">
-        <f>I176-G176</f>
+        <f t="shared" si="6"/>
         <v>0.80000000000000071</v>
       </c>
     </row>
@@ -7620,7 +7626,7 @@
         <v>41.1</v>
       </c>
       <c r="J177" s="1">
-        <f>I177-G177</f>
+        <f t="shared" si="6"/>
         <v>1.7700000000000031</v>
       </c>
     </row>
@@ -7648,7 +7654,7 @@
         <v>35.6</v>
       </c>
       <c r="J178" s="1">
-        <f>I178-G178</f>
+        <f t="shared" si="6"/>
         <v>1.5300000000000011</v>
       </c>
     </row>
@@ -7676,7 +7682,7 @@
         <v>27.8</v>
       </c>
       <c r="J179" s="1">
-        <f>I179-G179</f>
+        <f t="shared" si="6"/>
         <v>-5.4599999999999973</v>
       </c>
     </row>
@@ -7704,7 +7710,7 @@
         <v>58.6</v>
       </c>
       <c r="J180" s="1">
-        <f>I180-G180</f>
+        <f t="shared" si="6"/>
         <v>9.64</v>
       </c>
     </row>
@@ -7735,7 +7741,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="J181" s="1">
-        <f>I181-G181</f>
+        <f t="shared" si="6"/>
         <v>0.16000000000000369</v>
       </c>
     </row>
@@ -7766,7 +7772,7 @@
         <v>31.8</v>
       </c>
       <c r="J182" s="1">
-        <f>I182-G182</f>
+        <f t="shared" si="6"/>
         <v>-5.16</v>
       </c>
     </row>
@@ -7794,7 +7800,7 @@
         <v>39.5</v>
       </c>
       <c r="J183" s="1">
-        <f>I183-G183</f>
+        <f t="shared" si="6"/>
         <v>3.3500000000000014</v>
       </c>
     </row>
@@ -7910,7 +7916,7 @@
         <v>34.1</v>
       </c>
       <c r="J188" s="1">
-        <f>I188-G188</f>
+        <f t="shared" ref="J188:J197" si="7">I188-G188</f>
         <v>-1.1599999999999966</v>
       </c>
     </row>
@@ -7941,7 +7947,7 @@
         <v>43.6</v>
       </c>
       <c r="J189" s="1">
-        <f>I189-G189</f>
+        <f t="shared" si="7"/>
         <v>5.0799999999999983</v>
       </c>
     </row>
@@ -7969,7 +7975,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="J190" s="1">
-        <f>I190-G190</f>
+        <f t="shared" si="7"/>
         <v>-2.0700000000000003</v>
       </c>
     </row>
@@ -7997,7 +8003,7 @@
         <v>41.9</v>
       </c>
       <c r="J191" s="1">
-        <f>I191-G191</f>
+        <f t="shared" si="7"/>
         <v>8.4200000000000017</v>
       </c>
     </row>
@@ -8025,7 +8031,7 @@
         <v>37.9</v>
       </c>
       <c r="J192" s="1">
-        <f>I192-G192</f>
+        <f t="shared" si="7"/>
         <v>0.71000000000000085</v>
       </c>
     </row>
@@ -8056,7 +8062,7 @@
         <v>41.1</v>
       </c>
       <c r="J193" s="1">
-        <f>I193-G193</f>
+        <f t="shared" si="7"/>
         <v>5.9100000000000037</v>
       </c>
     </row>
@@ -8087,7 +8093,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="J194" s="1">
-        <f>I194-G194</f>
+        <f t="shared" si="7"/>
         <v>1.7900000000000027</v>
       </c>
     </row>
@@ -8115,7 +8121,7 @@
         <v>40.9</v>
       </c>
       <c r="J195" s="1">
-        <f>I195-G195</f>
+        <f t="shared" si="7"/>
         <v>2.75</v>
       </c>
     </row>
@@ -8146,7 +8152,7 @@
         <v>41.8</v>
       </c>
       <c r="J196" s="1">
-        <f>I196-G196</f>
+        <f t="shared" si="7"/>
         <v>5.43</v>
       </c>
     </row>
@@ -8174,7 +8180,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="J197" s="1">
-        <f>I197-G197</f>
+        <f t="shared" si="7"/>
         <v>1.4200000000000017</v>
       </c>
     </row>
@@ -8358,7 +8364,7 @@
         <v>37.299999999999997</v>
       </c>
       <c r="J204" s="1">
-        <f>I204-G204</f>
+        <f t="shared" ref="J204:J211" si="8">I204-G204</f>
         <v>0.62999999999999545</v>
       </c>
     </row>
@@ -8386,7 +8392,7 @@
         <v>45.8</v>
       </c>
       <c r="J205" s="1">
-        <f>I205-G205</f>
+        <f t="shared" si="8"/>
         <v>9.9499999999999957</v>
       </c>
     </row>
@@ -8414,7 +8420,7 @@
         <v>30.8</v>
       </c>
       <c r="J206" s="1">
-        <f>I206-G206</f>
+        <f t="shared" si="8"/>
         <v>-1.2699999999999996</v>
       </c>
     </row>
@@ -8442,7 +8448,7 @@
         <v>20.2</v>
       </c>
       <c r="J207" s="1">
-        <f>I207-G207</f>
+        <f t="shared" si="8"/>
         <v>-7.5</v>
       </c>
     </row>
@@ -8470,7 +8476,7 @@
         <v>27.8</v>
       </c>
       <c r="J208" s="1">
-        <f>I208-G208</f>
+        <f t="shared" si="8"/>
         <v>-10.569999999999997</v>
       </c>
     </row>
@@ -8498,7 +8504,7 @@
         <v>32.4</v>
       </c>
       <c r="J209" s="1">
-        <f>I209-G209</f>
+        <f t="shared" si="8"/>
         <v>4.4699999999999989</v>
       </c>
     </row>
@@ -8526,7 +8532,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J210" s="1">
-        <f>I210-G210</f>
+        <f t="shared" si="8"/>
         <v>1.8599999999999994</v>
       </c>
     </row>
@@ -8554,7 +8560,7 @@
         <v>32.4</v>
       </c>
       <c r="J211" s="1">
-        <f>I211-G211</f>
+        <f t="shared" si="8"/>
         <v>4.0299999999999976</v>
       </c>
     </row>
@@ -8735,7 +8741,7 @@
         <v>30.7</v>
       </c>
       <c r="J218" s="1">
-        <f>I218-G218</f>
+        <f t="shared" ref="J218:J224" si="9">I218-G218</f>
         <v>-9.9700000000000024</v>
       </c>
     </row>
@@ -8760,11 +8766,11 @@
       </c>
       <c r="H219"/>
       <c r="I219" s="4">
-        <v>36</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="J219" s="1">
-        <f>I219-G219</f>
-        <v>3.0399999999999991</v>
+        <f t="shared" si="9"/>
+        <v>1.240000000000002</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
@@ -8791,7 +8797,7 @@
         <v>20.8</v>
       </c>
       <c r="J220" s="1">
-        <f>I220-G220</f>
+        <f t="shared" si="9"/>
         <v>-12.309999999999999</v>
       </c>
     </row>
@@ -8819,7 +8825,7 @@
         <v>39.5</v>
       </c>
       <c r="J221" s="1">
-        <f>I221-G221</f>
+        <f t="shared" si="9"/>
         <v>5.57</v>
       </c>
     </row>
@@ -8850,7 +8856,7 @@
         <v>35.799999999999997</v>
       </c>
       <c r="J222" s="1">
-        <f>I222-G222</f>
+        <f t="shared" si="9"/>
         <v>2.2399999999999949</v>
       </c>
     </row>
@@ -8881,7 +8887,7 @@
         <v>33.6</v>
       </c>
       <c r="J223" s="1">
-        <f>I223-G223</f>
+        <f t="shared" si="9"/>
         <v>2.5600000000000023</v>
       </c>
     </row>
@@ -8909,7 +8915,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="J224" s="1">
-        <f>I224-G224</f>
+        <f t="shared" si="9"/>
         <v>5.389999999999997</v>
       </c>
     </row>
@@ -9037,7 +9043,7 @@
         <v>32</v>
       </c>
       <c r="J229" s="1">
-        <f>I229-G229</f>
+        <f t="shared" ref="J229:J238" si="10">I229-G229</f>
         <v>1.1099999999999994</v>
       </c>
     </row>
@@ -9065,7 +9071,7 @@
         <v>31.5</v>
       </c>
       <c r="J230" s="1">
-        <f>I230-G230</f>
+        <f t="shared" si="10"/>
         <v>1.129999999999999</v>
       </c>
     </row>
@@ -9093,7 +9099,7 @@
         <v>46.6</v>
       </c>
       <c r="J231" s="1">
-        <f>I231-G231</f>
+        <f t="shared" si="10"/>
         <v>9.3400000000000034</v>
       </c>
     </row>
@@ -9121,7 +9127,7 @@
         <v>28.9</v>
       </c>
       <c r="J232" s="1">
-        <f>I232-G232</f>
+        <f t="shared" si="10"/>
         <v>-0.58000000000000185</v>
       </c>
     </row>
@@ -9149,7 +9155,7 @@
         <v>45</v>
       </c>
       <c r="J233" s="1">
-        <f>I233-G233</f>
+        <f t="shared" si="10"/>
         <v>10.700000000000003</v>
       </c>
     </row>
@@ -9177,7 +9183,7 @@
         <v>32.4</v>
       </c>
       <c r="J234" s="1">
-        <f>I234-G234</f>
+        <f t="shared" si="10"/>
         <v>0.61999999999999744</v>
       </c>
     </row>
@@ -9205,7 +9211,7 @@
         <v>35.299999999999997</v>
       </c>
       <c r="J235" s="1">
-        <f>I235-G235</f>
+        <f t="shared" si="10"/>
         <v>5.5999999999999979</v>
       </c>
     </row>
@@ -9236,7 +9242,7 @@
         <v>44.2</v>
       </c>
       <c r="J236" s="1">
-        <f>I236-G236</f>
+        <f t="shared" si="10"/>
         <v>7.6099999999999994</v>
       </c>
     </row>
@@ -9264,7 +9270,7 @@
         <v>37.1</v>
       </c>
       <c r="J237" s="1">
-        <f>I237-G237</f>
+        <f t="shared" si="10"/>
         <v>4.8000000000000043</v>
       </c>
     </row>
@@ -9292,7 +9298,7 @@
         <v>35.6</v>
       </c>
       <c r="J238" s="1">
-        <f>I238-G238</f>
+        <f t="shared" si="10"/>
         <v>4.0400000000000027</v>
       </c>
     </row>
@@ -9345,7 +9351,7 @@
         <v>32.4</v>
       </c>
       <c r="J240" s="1">
-        <f>I240-G240</f>
+        <f t="shared" ref="J240:J249" si="11">I240-G240</f>
         <v>5.59</v>
       </c>
     </row>
@@ -9373,7 +9379,7 @@
         <v>37.9</v>
       </c>
       <c r="J241" s="1">
-        <f>I241-G241</f>
+        <f t="shared" si="11"/>
         <v>5.5300000000000011</v>
       </c>
     </row>
@@ -9404,7 +9410,7 @@
         <v>39.5</v>
       </c>
       <c r="J242" s="1">
-        <f>I242-G242</f>
+        <f t="shared" si="11"/>
         <v>5.2800000000000011</v>
       </c>
     </row>
@@ -9432,7 +9438,7 @@
         <v>32.4</v>
       </c>
       <c r="J243" s="1">
-        <f>I243-G243</f>
+        <f t="shared" si="11"/>
         <v>0.17999999999999972</v>
       </c>
     </row>
@@ -9460,7 +9466,7 @@
         <v>19.8</v>
       </c>
       <c r="J244" s="1">
-        <f>I244-G244</f>
+        <f t="shared" si="11"/>
         <v>-9.009999999999998</v>
       </c>
     </row>
@@ -9488,7 +9494,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="J245" s="1">
-        <f>I245-G245</f>
+        <f t="shared" si="11"/>
         <v>9.0399999999999956</v>
       </c>
     </row>
@@ -9516,7 +9522,7 @@
         <v>36</v>
       </c>
       <c r="J246" s="1">
-        <f>I246-G246</f>
+        <f t="shared" si="11"/>
         <v>2.740000000000002</v>
       </c>
     </row>
@@ -9544,7 +9550,7 @@
         <v>37.9</v>
       </c>
       <c r="J247" s="1">
-        <f>I247-G247</f>
+        <f t="shared" si="11"/>
         <v>4.1999999999999957</v>
       </c>
     </row>
@@ -9572,7 +9578,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="J248" s="1">
-        <f>I248-G248</f>
+        <f t="shared" si="11"/>
         <v>3.0399999999999991</v>
       </c>
     </row>
@@ -9597,11 +9603,11 @@
       </c>
       <c r="H249"/>
       <c r="I249" s="4">
-        <v>23.8</v>
+        <v>21.3</v>
       </c>
       <c r="J249" s="1">
-        <f>I249-G249</f>
-        <v>-8.870000000000001</v>
+        <f t="shared" si="11"/>
+        <v>-11.370000000000001</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
@@ -9650,7 +9656,7 @@
         <v>23</v>
       </c>
       <c r="J251" s="1">
-        <f>I251-G251</f>
+        <f t="shared" ref="J251:J260" si="12">I251-G251</f>
         <v>1.2199999999999989</v>
       </c>
     </row>
@@ -9678,7 +9684,7 @@
         <v>27.7</v>
       </c>
       <c r="J252" s="1">
-        <f>I252-G252</f>
+        <f t="shared" si="12"/>
         <v>-7.1900000000000013</v>
       </c>
     </row>
@@ -9706,7 +9712,7 @@
         <v>31.1</v>
       </c>
       <c r="J253" s="1">
-        <f>I253-G253</f>
+        <f t="shared" si="12"/>
         <v>1.1000000000000014</v>
       </c>
     </row>
@@ -9734,7 +9740,7 @@
         <v>36.9</v>
       </c>
       <c r="J254" s="1">
-        <f>I254-G254</f>
+        <f t="shared" si="12"/>
         <v>6.2299999999999969</v>
       </c>
     </row>
@@ -9762,7 +9768,7 @@
         <v>47.4</v>
       </c>
       <c r="J255" s="1">
-        <f>I255-G255</f>
+        <f t="shared" si="12"/>
         <v>11.25</v>
       </c>
     </row>
@@ -9790,7 +9796,7 @@
         <v>36.299999999999997</v>
       </c>
       <c r="J256" s="1">
-        <f>I256-G256</f>
+        <f t="shared" si="12"/>
         <v>5.7099999999999973</v>
       </c>
     </row>
@@ -9818,7 +9824,7 @@
         <v>23.8</v>
       </c>
       <c r="J257" s="1">
-        <f>I257-G257</f>
+        <f t="shared" si="12"/>
         <v>-5.98</v>
       </c>
     </row>
@@ -9846,7 +9852,7 @@
         <v>37.1</v>
       </c>
       <c r="J258" s="1">
-        <f>I258-G258</f>
+        <f t="shared" si="12"/>
         <v>6.5100000000000016</v>
       </c>
     </row>
@@ -9874,7 +9880,7 @@
         <v>54.5</v>
       </c>
       <c r="J259" s="1">
-        <f>I259-G259</f>
+        <f t="shared" si="12"/>
         <v>10.200000000000003</v>
       </c>
     </row>
@@ -9902,7 +9908,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="J260" s="1">
-        <f>I260-G260</f>
+        <f t="shared" si="12"/>
         <v>4.0599999999999987</v>
       </c>
     </row>
@@ -9949,11 +9955,11 @@
       </c>
       <c r="H262"/>
       <c r="I262" s="4">
-        <v>38.700000000000003</v>
+        <v>30.8</v>
       </c>
       <c r="J262" s="1">
         <f>I262-G262</f>
-        <v>7.9600000000000044</v>
+        <v>6.0000000000002274E-2</v>
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.2">
@@ -10002,11 +10008,11 @@
       </c>
       <c r="H264"/>
       <c r="I264" s="4">
-        <v>37</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="J264" s="1">
         <f>I264-G264</f>
-        <v>2.7800000000000011</v>
+        <v>0.57999999999999829</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.2">
@@ -10279,11 +10285,11 @@
       </c>
       <c r="H274"/>
       <c r="I274" s="4">
-        <v>31.4</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="J274" s="1">
         <f>I274-G274</f>
-        <v>8.59</v>
+        <v>11.390000000000004</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.2">
@@ -10600,7 +10606,7 @@
         <v>37.1</v>
       </c>
       <c r="J286" s="1">
-        <f>I286-G286</f>
+        <f t="shared" ref="J286:J293" si="13">I286-G286</f>
         <v>6.8800000000000026</v>
       </c>
     </row>
@@ -10628,7 +10634,7 @@
         <v>25.2</v>
       </c>
       <c r="J287" s="1">
-        <f>I287-G287</f>
+        <f t="shared" si="13"/>
         <v>-8.129999999999999</v>
       </c>
     </row>
@@ -10659,7 +10665,7 @@
         <v>26.2</v>
       </c>
       <c r="J288" s="1">
-        <f>I288-G288</f>
+        <f t="shared" si="13"/>
         <v>0.57000000000000028</v>
       </c>
     </row>
@@ -10687,7 +10693,7 @@
         <v>28.4</v>
       </c>
       <c r="J289" s="1">
-        <f>I289-G289</f>
+        <f t="shared" si="13"/>
         <v>3.4399999999999977</v>
       </c>
     </row>
@@ -10718,7 +10724,7 @@
         <v>37.9</v>
       </c>
       <c r="J290" s="1">
-        <f>I290-G290</f>
+        <f t="shared" si="13"/>
         <v>5.68</v>
       </c>
     </row>
@@ -10746,7 +10752,7 @@
         <v>30.4</v>
       </c>
       <c r="J291" s="1">
-        <f>I291-G291</f>
+        <f t="shared" si="13"/>
         <v>0.76999999999999957</v>
       </c>
     </row>
@@ -10795,7 +10801,13 @@
         <v>35.630000000000003</v>
       </c>
       <c r="H293"/>
-      <c r="I293" s="4"/>
+      <c r="I293" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="J293" s="1">
+        <f t="shared" si="13"/>
+        <v>-7.0300000000000011</v>
+      </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294">
@@ -10839,7 +10851,13 @@
         <v>20.3</v>
       </c>
       <c r="H295"/>
-      <c r="I295" s="4"/>
+      <c r="I295" s="4">
+        <v>27.7</v>
+      </c>
+      <c r="J295" s="1">
+        <f>I295-G295</f>
+        <v>7.3999999999999986</v>
+      </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296">
@@ -10861,7 +10879,13 @@
         <v>37.19</v>
       </c>
       <c r="H296"/>
-      <c r="I296" s="4"/>
+      <c r="I296" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="J296" s="1">
+        <f>I296-G296</f>
+        <v>-31.889999999999997</v>
+      </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297">
@@ -10884,11 +10908,11 @@
       </c>
       <c r="H297"/>
       <c r="I297" s="4">
-        <v>18.100000000000001</v>
+        <v>29.8</v>
       </c>
       <c r="J297" s="1">
         <f>I297-G297</f>
-        <v>-4.639999999999997</v>
+        <v>7.0600000000000023</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
@@ -11663,7 +11687,13 @@
         <v>28.15</v>
       </c>
       <c r="H327"/>
-      <c r="I327" s="4"/>
+      <c r="I327" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="J327" s="1">
+        <f>I327-G327</f>
+        <v>-13.849999999999998</v>
+      </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328">
@@ -12479,7 +12509,13 @@
         <v>17.04</v>
       </c>
       <c r="H360"/>
-      <c r="I360" s="4"/>
+      <c r="I360" s="4">
+        <v>44.7</v>
+      </c>
+      <c r="J360" s="1">
+        <f>I360-G360</f>
+        <v>27.660000000000004</v>
+      </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361">

</xml_diff>

<commit_message>
correct projections for error
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2545EA52-FAF3-8248-BC74-29E507007C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E64BDC-9AFE-AA43-9FEC-33509A7603C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="23780" windowHeight="14500" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
@@ -11090,7 +11090,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C545" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E556" sqref="E556"/>
+      <selection pane="bottomRight" activeCell="I554" sqref="I554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11124,7 +11124,7 @@
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="3" t="s">

</xml_diff>

<commit_message>
Round 20 post TLT + fixtures update
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9403C8BE-57C4-6840-831D-E52A788BAD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69FCB29-4A1B-1F4F-8445-11E7CBD4687C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="1000" windowWidth="23780" windowHeight="14500" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="23780" windowHeight="14500" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -2381,6 +2381,206 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>515140</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>118180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>515500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>118180</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EADEB2A-F86D-685A-80A3-88BB64A95154}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1340640" y="562680"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EADEB2A-F86D-685A-80A3-88BB64A95154}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1336320" y="558360"/>
+              <a:ext cx="9000" cy="9000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>519120</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>93700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>520920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>93700</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338E2C69-46AA-212F-71E0-41D2458E9B18}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2805120" y="538200"/>
+            <a:ext cx="1800" cy="9360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338E2C69-46AA-212F-71E0-41D2458E9B18}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2800800" y="533880"/>
+              <a:ext cx="10440" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>968380</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>968740</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2460</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6397F04-4DFE-0485-EDB4-21943740BA83}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1793880" y="650160"/>
+            <a:ext cx="360" cy="1800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6397F04-4DFE-0485-EDB4-21943740BA83}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1789560" y="645840"/>
+              <a:ext cx="9000" cy="10440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -3380,19 +3580,19 @@
         </row>
         <row r="36">
           <cell r="C36">
-            <v>43.5</v>
+            <v>41.1</v>
           </cell>
           <cell r="D36">
             <v>43</v>
           </cell>
           <cell r="E36">
-            <v>0.4</v>
+            <v>-2</v>
           </cell>
           <cell r="F36">
             <v>44</v>
           </cell>
           <cell r="G36">
-            <v>-0.5</v>
+            <v>-2.9</v>
           </cell>
           <cell r="H36" t="str">
             <v>DANE</v>
@@ -4076,19 +4276,19 @@
         </row>
         <row r="60">
           <cell r="C60">
-            <v>41.9</v>
+            <v>30.8</v>
           </cell>
           <cell r="D60">
             <v>30</v>
           </cell>
           <cell r="E60">
-            <v>11.7</v>
+            <v>0.7</v>
           </cell>
           <cell r="F60">
             <v>32</v>
           </cell>
           <cell r="G60">
-            <v>9.9</v>
+            <v>-1.2</v>
           </cell>
           <cell r="H60" t="str">
             <v>kieran</v>
@@ -4221,19 +4421,19 @@
         </row>
         <row r="65">
           <cell r="C65">
-            <v>67</v>
+            <v>71.3</v>
           </cell>
           <cell r="D65">
             <v>64</v>
           </cell>
           <cell r="E65">
-            <v>2.8</v>
+            <v>7.1</v>
           </cell>
           <cell r="F65">
             <v>77</v>
           </cell>
           <cell r="G65">
-            <v>-10</v>
+            <v>-5.7</v>
           </cell>
           <cell r="H65" t="str">
             <v>PAYNE</v>
@@ -5816,19 +6016,19 @@
         </row>
         <row r="120">
           <cell r="C120">
-            <v>18</v>
+            <v>45.8</v>
           </cell>
           <cell r="D120">
             <v>33</v>
           </cell>
           <cell r="E120">
-            <v>-15.4</v>
+            <v>12.4</v>
           </cell>
           <cell r="F120">
             <v>46</v>
           </cell>
           <cell r="G120">
-            <v>-28</v>
+            <v>-0.2</v>
           </cell>
           <cell r="H120" t="str">
             <v>lachlan</v>
@@ -6512,19 +6712,19 @@
         </row>
         <row r="144">
           <cell r="C144">
-            <v>14.3</v>
+            <v>35.799999999999997</v>
           </cell>
           <cell r="D144">
             <v>30</v>
           </cell>
           <cell r="E144">
-            <v>-16</v>
+            <v>5.5</v>
           </cell>
           <cell r="F144">
             <v>55</v>
           </cell>
           <cell r="G144">
-            <v>-40.700000000000003</v>
+            <v>-19.3</v>
           </cell>
           <cell r="H144" t="str">
             <v>Brodie</v>
@@ -6918,19 +7118,19 @@
         </row>
         <row r="158">
           <cell r="C158">
-            <v>58.9</v>
+            <v>62.9</v>
           </cell>
           <cell r="D158">
             <v>54</v>
           </cell>
           <cell r="E158">
-            <v>5.3</v>
+            <v>9.1999999999999993</v>
           </cell>
           <cell r="F158">
             <v>48</v>
           </cell>
           <cell r="G158">
-            <v>10.9</v>
+            <v>14.9</v>
           </cell>
           <cell r="H158" t="str">
             <v>latrell</v>
@@ -7614,19 +7814,19 @@
         </row>
         <row r="182">
           <cell r="C182">
-            <v>34</v>
+            <v>30.8</v>
           </cell>
           <cell r="D182">
+            <v>30</v>
+          </cell>
+          <cell r="E182">
+            <v>0.7</v>
+          </cell>
+          <cell r="F182">
             <v>32</v>
           </cell>
-          <cell r="E182">
-            <v>2.4</v>
-          </cell>
-          <cell r="F182">
-            <v>27</v>
-          </cell>
           <cell r="G182">
-            <v>7</v>
+            <v>-1.2</v>
           </cell>
           <cell r="H182" t="str">
             <v>jack</v>
@@ -8629,19 +8829,19 @@
         </row>
         <row r="217">
           <cell r="C217">
-            <v>36</v>
+            <v>31.5</v>
           </cell>
           <cell r="D217">
             <v>28</v>
           </cell>
           <cell r="E217">
-            <v>7.7</v>
+            <v>3.2</v>
           </cell>
           <cell r="F217">
             <v>32</v>
           </cell>
           <cell r="G217">
-            <v>4</v>
+            <v>-0.5</v>
           </cell>
           <cell r="H217" t="str">
             <v>FONUA</v>
@@ -9815,19 +10015,19 @@
         </row>
         <row r="258">
           <cell r="C258">
-            <v>55.3</v>
+            <v>48.8</v>
           </cell>
           <cell r="D258">
             <v>45</v>
           </cell>
           <cell r="E258">
-            <v>10.5</v>
+            <v>4</v>
           </cell>
           <cell r="F258">
             <v>40</v>
           </cell>
           <cell r="G258">
-            <v>15.3</v>
+            <v>8.8000000000000007</v>
           </cell>
           <cell r="H258" t="str">
             <v>kurt</v>
@@ -10774,6 +10974,90 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-07-16T13:08:29.197"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-07-16T13:08:35.884"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5 22 23936,'-3'2'0,"1"0"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="309">0 1 24575,'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="459">0 1 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-07-16T13:08:37.328"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 5 23235,'0'-3'0,"0"1"0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165">1 0 24575,'0'0'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11096,10 +11380,10 @@
   <dimension ref="A1:K562"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11192,11 +11476,11 @@
       <c r="H3"/>
       <c r="I3" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B3,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>67</v>
+        <v>71.3</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J66" si="0">I3-G3</f>
-        <v>2.3299999999999983</v>
+        <v>6.6299999999999955</v>
       </c>
       <c r="K3"/>
     </row>
@@ -11576,11 +11860,11 @@
       <c r="H16"/>
       <c r="I16" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B16,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>58.9</v>
+        <v>62.9</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>4.8299999999999983</v>
+        <v>8.8299999999999983</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -13763,11 +14047,11 @@
       <c r="H91"/>
       <c r="I91" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B91,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>43.5</v>
+        <v>41.1</v>
       </c>
       <c r="J91" s="1">
         <f t="shared" si="1"/>
-        <v>9.0000000000003411E-2</v>
+        <v>-2.3099999999999952</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
@@ -14465,11 +14749,11 @@
       <c r="H115"/>
       <c r="I115" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B115,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>18</v>
+        <v>45.8</v>
       </c>
       <c r="J115" s="1">
         <f t="shared" si="1"/>
-        <v>-15.630000000000003</v>
+        <v>12.169999999999995</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -15110,11 +15394,11 @@
       <c r="H137"/>
       <c r="I137" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B137,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>55.3</v>
+        <v>48.8</v>
       </c>
       <c r="J137" s="1">
         <f t="shared" si="2"/>
-        <v>10.189999999999998</v>
+        <v>3.6899999999999977</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
@@ -18681,11 +18965,11 @@
       <c r="H260"/>
       <c r="I260" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B260,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>36</v>
+        <v>31.5</v>
       </c>
       <c r="J260" s="1">
         <f t="shared" si="4"/>
-        <v>7.48</v>
+        <v>2.9800000000000004</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.2">
@@ -19530,11 +19814,11 @@
       <c r="H290"/>
       <c r="I290" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B290,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>34</v>
+        <v>30.8</v>
       </c>
       <c r="J290" s="1">
         <f t="shared" si="4"/>
-        <v>2.2199999999999989</v>
+        <v>-0.98000000000000043</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.2">
@@ -19671,11 +19955,11 @@
       </c>
       <c r="I295" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B295,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>41.9</v>
+        <v>30.8</v>
       </c>
       <c r="J295" s="1">
         <f t="shared" si="4"/>
-        <v>11.529999999999998</v>
+        <v>0.42999999999999972</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -19990,11 +20274,11 @@
       <c r="H306"/>
       <c r="I306" s="4">
         <f>INDEX([1]CleanedBook4!$C$2:$K$290,MATCH(B306,[1]CleanedBook4!$K$2:$K$290,0),1)</f>
-        <v>14.3</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="J306" s="1">
         <f t="shared" si="4"/>
-        <v>-16.22</v>
+        <v>5.2799999999999976</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.2">
@@ -26848,5 +27132,6 @@
     <sortCondition descending="1" ref="F1:F535"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rnd 23 2nd update
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C2D53-335D-574C-9EB6-080F083B6AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD5880-F1E1-A54C-879E-2C2EB045E087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="500" windowWidth="20780" windowHeight="13380" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
@@ -2612,7 +2612,7 @@
       <sheetName val="reorganized_player_data (2)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="2">
           <cell r="C2">
             <v>45</v>
@@ -11404,10 +11404,10 @@
   <dimension ref="A1:K569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C142" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C247" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B144" sqref="B144"/>
+      <selection pane="bottomRight" activeCell="I259" sqref="I259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18964,10 +18964,13 @@
         <v>20.89</v>
       </c>
       <c r="H259"/>
-      <c r="I259" s="4"/>
+      <c r="I259" s="4">
+        <f>INDEX('[1]reorganized_player_data (2)'!$C$2:$K$290,MATCH(B259,'[1]reorganized_player_data (2)'!$K$2:$K$290,0),1)</f>
+        <v>40.6</v>
+      </c>
       <c r="J259" s="1">
         <f t="shared" ref="J259:J322" si="4">I259-G259</f>
-        <v>-20.89</v>
+        <v>19.71</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update init_heroku_db file for addition of Injured + bye_round_grading
</commit_message>
<xml_diff>
--- a/NRL_stats.xlsx
+++ b/NRL_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator_deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD5880-F1E1-A54C-879E-2C2EB045E087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8862F963-70BB-F84B-931D-A45EC84C3746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="500" windowWidth="20780" windowHeight="13380" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="602">
   <si>
     <t>Price</t>
   </si>
@@ -1839,6 +1839,12 @@
   </si>
   <si>
     <t>LJ Nonu</t>
+  </si>
+  <si>
+    <t>Bye Round Grading</t>
+  </si>
+  <si>
+    <t>Injured</t>
   </si>
 </sst>
 </file>
@@ -2333,7 +2339,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2343,6 +2349,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -11401,13 +11410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1841C9-D21C-2040-9467-2F510B1F6134}">
-  <dimension ref="A1:K569"/>
+  <dimension ref="A1:L569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C247" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I259" sqref="I259"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11419,7 +11428,7 @@
     <col min="10" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -11447,9 +11456,14 @@
       <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K1" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11477,8 +11491,11 @@
         <f>I2-G2</f>
         <v>6.4000000000000057</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11506,9 +11523,11 @@
         <f t="shared" ref="J3:J66" si="0">I3-G3</f>
         <v>2.6399999999999935</v>
       </c>
-      <c r="K3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11536,8 +11555,11 @@
         <f t="shared" si="0"/>
         <v>4.4899999999999949</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -11562,8 +11584,11 @@
         <f t="shared" si="0"/>
         <v>-62.37</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11591,8 +11616,11 @@
         <f t="shared" si="0"/>
         <v>2.9100000000000037</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -11623,8 +11651,11 @@
         <f t="shared" si="0"/>
         <v>8.4600000000000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -11652,8 +11683,11 @@
         <f t="shared" si="0"/>
         <v>2.8400000000000034</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -11681,8 +11715,11 @@
         <f t="shared" si="0"/>
         <v>2.3699999999999974</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -11713,8 +11750,14 @@
         <f t="shared" si="0"/>
         <v>0.60999999999999943</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -11742,8 +11785,11 @@
         <f t="shared" si="0"/>
         <v>-51.04</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -11771,8 +11817,14 @@
         <f t="shared" si="0"/>
         <v>4.9699999999999989</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -11800,8 +11852,11 @@
         <f t="shared" si="0"/>
         <v>9.240000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -11829,8 +11884,11 @@
         <f t="shared" si="0"/>
         <v>3.4399999999999977</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -11858,8 +11916,11 @@
         <f t="shared" si="0"/>
         <v>-52.74</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -11887,8 +11948,11 @@
         <f t="shared" si="0"/>
         <v>3.3299999999999983</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -11916,8 +11980,11 @@
         <f t="shared" si="0"/>
         <v>-54</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -11942,8 +12009,11 @@
         <f t="shared" si="0"/>
         <v>-50.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -11971,8 +12041,11 @@
         <f t="shared" si="0"/>
         <v>6.5399999999999991</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -12000,8 +12073,11 @@
         <f t="shared" si="0"/>
         <v>2.2900000000000063</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -12032,8 +12108,11 @@
         <f t="shared" si="0"/>
         <v>4.5100000000000051</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -12061,8 +12140,11 @@
         <f t="shared" si="0"/>
         <v>3.2899999999999991</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -12090,8 +12172,11 @@
         <f t="shared" si="0"/>
         <v>-9.64</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -12119,8 +12204,11 @@
         <f t="shared" si="0"/>
         <v>-47.11</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -12151,8 +12239,11 @@
         <f t="shared" si="0"/>
         <v>4.269999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -12180,8 +12271,11 @@
         <f t="shared" si="0"/>
         <v>0.71000000000000085</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -12212,8 +12306,11 @@
         <f t="shared" si="0"/>
         <v>8.11</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -12241,8 +12338,11 @@
         <f t="shared" si="0"/>
         <v>8.2899999999999991</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -12270,8 +12370,11 @@
         <f t="shared" si="0"/>
         <v>1.1099999999999994</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -12299,8 +12402,11 @@
         <f t="shared" si="0"/>
         <v>0.46999999999999886</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -12325,8 +12431,11 @@
         <f t="shared" si="0"/>
         <v>-49.78</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -12354,8 +12463,11 @@
         <f t="shared" si="0"/>
         <v>0.68999999999999773</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -12380,8 +12492,11 @@
         <f t="shared" si="0"/>
         <v>-51.85</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -12409,8 +12524,11 @@
         <f t="shared" si="0"/>
         <v>7.0200000000000031</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -12438,8 +12556,11 @@
         <f t="shared" si="0"/>
         <v>7.3599999999999994</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -12467,8 +12588,11 @@
         <f t="shared" si="0"/>
         <v>9.6899999999999977</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -12499,8 +12623,11 @@
         <f t="shared" si="0"/>
         <v>2.6099999999999994</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -12528,8 +12655,11 @@
         <f t="shared" si="0"/>
         <v>9.1999999999999957</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -12557,8 +12687,11 @@
         <f t="shared" si="0"/>
         <v>5.4699999999999989</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -12586,8 +12719,11 @@
         <f t="shared" si="0"/>
         <v>12.299999999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -12612,8 +12748,11 @@
         <f t="shared" si="0"/>
         <v>-47.63</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -12641,8 +12780,11 @@
         <f t="shared" si="0"/>
         <v>0.67000000000000171</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -12670,8 +12812,11 @@
         <f t="shared" si="0"/>
         <v>-5.4600000000000009</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -12699,8 +12844,14 @@
         <f t="shared" si="0"/>
         <v>-6.3500000000000014</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -12731,8 +12882,11 @@
         <f t="shared" si="0"/>
         <v>5.259999999999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -12760,8 +12914,11 @@
         <f t="shared" si="0"/>
         <v>6.1600000000000037</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -12789,8 +12946,11 @@
         <f t="shared" si="0"/>
         <v>11.030000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -12818,8 +12978,11 @@
         <f t="shared" si="0"/>
         <v>3.4500000000000028</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -12847,8 +13010,11 @@
         <f t="shared" si="0"/>
         <v>-1.9400000000000048</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -12879,8 +13045,11 @@
         <f t="shared" si="0"/>
         <v>1.009999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -12908,8 +13077,11 @@
         <f t="shared" si="0"/>
         <v>-0.75</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -12937,8 +13109,11 @@
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -12966,8 +13141,11 @@
         <f t="shared" si="0"/>
         <v>-1.0599999999999952</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -12995,8 +13173,11 @@
         <f t="shared" si="0"/>
         <v>5.3299999999999983</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -13027,8 +13208,11 @@
         <f t="shared" si="0"/>
         <v>2.0399999999999991</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -13056,8 +13240,11 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -13082,8 +13269,11 @@
         <f t="shared" si="0"/>
         <v>-43.48</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -13108,8 +13298,11 @@
         <f t="shared" si="0"/>
         <v>-45.7</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -13137,8 +13330,11 @@
         <f t="shared" si="0"/>
         <v>10.93</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -13169,8 +13365,11 @@
         <f t="shared" si="0"/>
         <v>5.9399999999999977</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -13195,8 +13394,11 @@
         <f t="shared" si="0"/>
         <v>-52.67</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -13227,8 +13429,11 @@
         <f t="shared" si="0"/>
         <v>7.5799999999999983</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -13253,8 +13458,11 @@
         <f t="shared" si="0"/>
         <v>-45.93</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -13279,8 +13487,11 @@
         <f t="shared" si="0"/>
         <v>-39.11</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -13308,8 +13519,11 @@
         <f t="shared" si="0"/>
         <v>-0.62000000000000455</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -13337,8 +13551,11 @@
         <f t="shared" si="0"/>
         <v>0.24000000000000199</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1</v>
       </c>
@@ -13366,8 +13583,11 @@
         <f t="shared" ref="J67:J130" si="1">I67-G67</f>
         <v>6.7000000000000028</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -13395,8 +13615,11 @@
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
@@ -13421,8 +13644,11 @@
         <f t="shared" si="1"/>
         <v>-30.44</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -13450,8 +13676,11 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -13479,8 +13708,11 @@
         <f t="shared" si="1"/>
         <v>-0.24000000000000199</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -13508,8 +13740,11 @@
         <f t="shared" si="1"/>
         <v>3.9899999999999949</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -13537,8 +13772,11 @@
         <f t="shared" si="1"/>
         <v>7.07</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -13563,8 +13801,11 @@
         <f t="shared" si="1"/>
         <v>-38.89</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -13592,8 +13833,11 @@
         <f t="shared" si="1"/>
         <v>-46.3</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -13621,8 +13865,11 @@
         <f t="shared" si="1"/>
         <v>5.6400000000000006</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -13653,8 +13900,11 @@
         <f t="shared" si="1"/>
         <v>0.19999999999999574</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -13682,8 +13932,11 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999972</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -13711,8 +13964,11 @@
         <f t="shared" si="1"/>
         <v>5.019999999999996</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -13743,8 +13999,11 @@
         <f t="shared" si="1"/>
         <v>7.4699999999999989</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -13775,8 +14034,11 @@
         <f t="shared" si="1"/>
         <v>4.1700000000000017</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -13807,8 +14069,11 @@
         <f t="shared" si="1"/>
         <v>-7.6600000000000037</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -13836,8 +14101,11 @@
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -13865,8 +14133,11 @@
         <f t="shared" si="1"/>
         <v>1.5600000000000023</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
@@ -13894,8 +14165,11 @@
         <f t="shared" si="1"/>
         <v>9.8500000000000014</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -13926,8 +14200,11 @@
         <f t="shared" si="1"/>
         <v>7.509999999999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -13955,8 +14232,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -13984,8 +14264,11 @@
         <f t="shared" si="1"/>
         <v>3.9099999999999966</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -14013,8 +14296,11 @@
         <f t="shared" si="1"/>
         <v>-3.279999999999994</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -14042,8 +14328,11 @@
         <f t="shared" si="1"/>
         <v>6.2100000000000009</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -14071,8 +14360,11 @@
         <f t="shared" si="1"/>
         <v>3.8900000000000006</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -14103,8 +14395,11 @@
         <f t="shared" si="1"/>
         <v>7.230000000000004</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -14135,8 +14430,11 @@
         <f t="shared" si="1"/>
         <v>5.4200000000000017</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -14164,8 +14462,11 @@
         <f t="shared" si="1"/>
         <v>-43.85</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -14193,8 +14494,11 @@
         <f t="shared" si="1"/>
         <v>-0.92999999999999972</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
@@ -14219,8 +14523,11 @@
         <f t="shared" si="1"/>
         <v>-39.33</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -14248,8 +14555,11 @@
         <f t="shared" si="1"/>
         <v>-3.1099999999999994</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1</v>
       </c>
@@ -14274,8 +14584,11 @@
         <f t="shared" si="1"/>
         <v>-44.15</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1</v>
       </c>
@@ -14303,8 +14616,11 @@
         <f t="shared" si="1"/>
         <v>7.980000000000004</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
@@ -14332,8 +14648,11 @@
         <f t="shared" si="1"/>
         <v>-42.37</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1</v>
       </c>
@@ -14361,8 +14680,11 @@
         <f t="shared" si="1"/>
         <v>-3.1400000000000006</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1</v>
       </c>
@@ -14390,8 +14712,11 @@
         <f t="shared" si="1"/>
         <v>9.1900000000000048</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1</v>
       </c>
@@ -14419,8 +14744,11 @@
         <f t="shared" si="1"/>
         <v>0.49000000000000199</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1</v>
       </c>
@@ -14448,8 +14776,11 @@
         <f t="shared" si="1"/>
         <v>-3.1999999999999957</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1</v>
       </c>
@@ -14477,8 +14808,11 @@
         <f t="shared" si="1"/>
         <v>5.1200000000000045</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -14506,8 +14840,11 @@
         <f t="shared" si="1"/>
         <v>-7.259999999999998</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>1</v>
       </c>
@@ -14538,8 +14875,14 @@
         <f t="shared" si="1"/>
         <v>3.4799999999999969</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <v>4</v>
+      </c>
+      <c r="L107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1</v>
       </c>
@@ -14567,8 +14910,11 @@
         <f t="shared" si="1"/>
         <v>4.0600000000000023</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1</v>
       </c>
@@ -14596,8 +14942,11 @@
         <f t="shared" si="1"/>
         <v>13.779999999999994</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1</v>
       </c>
@@ -14625,8 +14974,11 @@
         <f t="shared" si="1"/>
         <v>-5.6400000000000006</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1</v>
       </c>
@@ -14651,8 +15003,11 @@
         <f t="shared" si="1"/>
         <v>-40.369999999999997</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1</v>
       </c>
@@ -14680,6 +15035,9 @@
         <f t="shared" si="1"/>
         <v>11.299999999999997</v>
       </c>
+      <c r="K112">
+        <v>4</v>
+      </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113">
@@ -14709,6 +15067,9 @@
         <f t="shared" si="1"/>
         <v>9.7299999999999969</v>
       </c>
+      <c r="K113">
+        <v>4</v>
+      </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114">
@@ -14741,6 +15102,9 @@
         <f t="shared" si="1"/>
         <v>-0.57000000000000028</v>
       </c>
+      <c r="K114">
+        <v>4</v>
+      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
@@ -14769,6 +15133,9 @@
       <c r="J115" s="1">
         <f t="shared" si="1"/>
         <v>-6.740000000000002</v>
+      </c>
+      <c r="K115">
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -14796,6 +15163,9 @@
         <f t="shared" si="1"/>
         <v>-18.809999999999999</v>
       </c>
+      <c r="K116">
+        <v>4</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117">
@@ -14822,6 +15192,9 @@
         <f t="shared" si="1"/>
         <v>-38.07</v>
       </c>
+      <c r="K117">
+        <v>4</v>
+      </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
@@ -14851,6 +15224,9 @@
         <f t="shared" si="1"/>
         <v>-45.85</v>
       </c>
+      <c r="K118">
+        <v>4</v>
+      </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119">
@@ -14880,6 +15256,9 @@
         <f t="shared" si="1"/>
         <v>-0.14000000000000057</v>
       </c>
+      <c r="K119">
+        <v>4</v>
+      </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120">
@@ -14909,6 +15288,9 @@
         <f t="shared" si="1"/>
         <v>-4.6499999999999986</v>
       </c>
+      <c r="K120">
+        <v>4</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
@@ -14937,6 +15319,9 @@
       <c r="J121" s="1">
         <f t="shared" si="1"/>
         <v>-1.1199999999999974</v>
+      </c>
+      <c r="K121">
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -14967,6 +15352,9 @@
         <f t="shared" si="1"/>
         <v>-38.590000000000003</v>
       </c>
+      <c r="K122">
+        <v>4</v>
+      </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123">
@@ -14996,6 +15384,9 @@
         <f t="shared" si="1"/>
         <v>0.17000000000000171</v>
       </c>
+      <c r="K123">
+        <v>4</v>
+      </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
@@ -15027,6 +15418,9 @@
       <c r="J124" s="1">
         <f t="shared" si="1"/>
         <v>-4.2200000000000024</v>
+      </c>
+      <c r="K124">
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
@@ -15054,7 +15448,9 @@
         <f t="shared" si="1"/>
         <v>-39.26</v>
       </c>
-      <c r="K125"/>
+      <c r="K125">
+        <v>4</v>
+      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126">
@@ -15084,6 +15480,9 @@
         <f t="shared" si="1"/>
         <v>-2.2199999999999989</v>
       </c>
+      <c r="K126">
+        <v>4</v>
+      </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
@@ -15116,6 +15515,9 @@
         <f t="shared" si="1"/>
         <v>1.4899999999999949</v>
       </c>
+      <c r="K127">
+        <v>4</v>
+      </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
@@ -15148,8 +15550,11 @@
         <f t="shared" si="1"/>
         <v>5.18</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1</v>
       </c>
@@ -15174,8 +15579,11 @@
         <f t="shared" si="1"/>
         <v>-18.52</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1</v>
       </c>
@@ -15203,8 +15611,11 @@
         <f t="shared" si="1"/>
         <v>-3.4099999999999966</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1</v>
       </c>
@@ -15232,8 +15643,11 @@
         <f t="shared" ref="J131:J194" si="2">I131-G131</f>
         <v>-36.520000000000003</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1</v>
       </c>
@@ -15264,8 +15678,11 @@
         <f t="shared" si="2"/>
         <v>-2.3799999999999955</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1</v>
       </c>
@@ -15296,8 +15713,11 @@
         <f t="shared" si="2"/>
         <v>1.2999999999999972</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1</v>
       </c>
@@ -15325,8 +15745,11 @@
         <f t="shared" si="2"/>
         <v>2.1499999999999986</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1</v>
       </c>
@@ -15354,8 +15777,11 @@
         <f t="shared" si="2"/>
         <v>1.8900000000000006</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1</v>
       </c>
@@ -15386,8 +15812,11 @@
         <f t="shared" si="2"/>
         <v>-0.40999999999999659</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1</v>
       </c>
@@ -15415,8 +15844,11 @@
         <f t="shared" si="2"/>
         <v>1.4399999999999977</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>1</v>
       </c>
@@ -15444,8 +15876,11 @@
         <f t="shared" si="2"/>
         <v>6.6099999999999994</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>1</v>
       </c>
@@ -15476,8 +15911,11 @@
         <f t="shared" si="2"/>
         <v>-2.9699999999999989</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>1</v>
       </c>
@@ -15505,8 +15943,11 @@
         <f t="shared" si="2"/>
         <v>-37.56</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1</v>
       </c>
@@ -15534,8 +15975,11 @@
         <f t="shared" si="2"/>
         <v>-1.2100000000000009</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1</v>
       </c>
@@ -15563,8 +16007,11 @@
         <f t="shared" si="2"/>
         <v>-1.3399999999999963</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1</v>
       </c>
@@ -15589,8 +16036,11 @@
         <f t="shared" si="2"/>
         <v>-45.78</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1</v>
       </c>
@@ -15617,6 +16067,9 @@
       <c r="J144" s="1">
         <f t="shared" si="2"/>
         <v>-5.009999999999998</v>
+      </c>
+      <c r="K144">
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
@@ -15644,6 +16097,9 @@
         <f t="shared" si="2"/>
         <v>-34.590000000000003</v>
       </c>
+      <c r="K145">
+        <v>4</v>
+      </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
@@ -15673,6 +16129,9 @@
         <f t="shared" si="2"/>
         <v>11.549999999999997</v>
       </c>
+      <c r="K146">
+        <v>4</v>
+      </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
@@ -15701,6 +16160,9 @@
       <c r="J147" s="1">
         <f t="shared" si="2"/>
         <v>7.3399999999999963</v>
+      </c>
+      <c r="K147">
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
@@ -15728,6 +16190,9 @@
         <f t="shared" si="2"/>
         <v>-37.26</v>
       </c>
+      <c r="K148">
+        <v>4</v>
+      </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
@@ -15757,6 +16222,9 @@
         <f t="shared" si="2"/>
         <v>-4.990000000000002</v>
       </c>
+      <c r="K149">
+        <v>4</v>
+      </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
@@ -15786,6 +16254,9 @@
         <f t="shared" si="2"/>
         <v>-9.4600000000000009</v>
       </c>
+      <c r="K150">
+        <v>4</v>
+      </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
@@ -15815,6 +16286,9 @@
         <f t="shared" si="2"/>
         <v>-4.2199999999999989</v>
       </c>
+      <c r="K151">
+        <v>4</v>
+      </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
@@ -15844,6 +16318,9 @@
         <f t="shared" si="2"/>
         <v>-0.43999999999999773</v>
       </c>
+      <c r="K152">
+        <v>4</v>
+      </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -15873,6 +16350,9 @@
         <f t="shared" si="2"/>
         <v>-6.1900000000000048</v>
       </c>
+      <c r="K153">
+        <v>4</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
@@ -15905,6 +16385,9 @@
         <f t="shared" si="2"/>
         <v>-16.93</v>
       </c>
+      <c r="K154">
+        <v>4</v>
+      </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
@@ -15934,6 +16417,9 @@
         <f t="shared" si="2"/>
         <v>3.7600000000000051</v>
       </c>
+      <c r="K155">
+        <v>4</v>
+      </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
@@ -15966,6 +16452,9 @@
         <f t="shared" si="2"/>
         <v>1.1299999999999955</v>
       </c>
+      <c r="K156">
+        <v>4</v>
+      </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
@@ -15995,6 +16484,9 @@
         <f t="shared" si="2"/>
         <v>-2.6499999999999986</v>
       </c>
+      <c r="K157">
+        <v>4</v>
+      </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
@@ -16026,6 +16518,9 @@
       <c r="J158" s="1">
         <f t="shared" si="2"/>
         <v>7.5300000000000011</v>
+      </c>
+      <c r="K158">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
@@ -16056,7 +16551,9 @@
         <f t="shared" si="2"/>
         <v>-36.81</v>
       </c>
-      <c r="K159"/>
+      <c r="K159">
+        <v>4</v>
+      </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
@@ -16089,8 +16586,11 @@
         <f t="shared" si="2"/>
         <v>9.9999999999980105E-3</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K160">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>1</v>
       </c>
@@ -16118,8 +16618,11 @@
         <f t="shared" si="2"/>
         <v>-8.509999999999998</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1</v>
       </c>
@@ -16147,8 +16650,11 @@
         <f t="shared" si="2"/>
         <v>-9.9999999999994316E-2</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1</v>
       </c>
@@ -16176,8 +16682,11 @@
         <f t="shared" si="2"/>
         <v>-13.380000000000003</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K163">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1</v>
       </c>
@@ -16208,8 +16717,11 @@
         <f t="shared" si="2"/>
         <v>-4.8700000000000045</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1</v>
       </c>
@@ -16237,8 +16749,11 @@
         <f t="shared" si="2"/>
         <v>-6.3999999999999986</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>1</v>
       </c>
@@ -16269,8 +16784,11 @@
         <f t="shared" si="2"/>
         <v>-6.5300000000000011</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1</v>
       </c>
@@ -16298,8 +16816,11 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1</v>
       </c>
@@ -16327,8 +16848,11 @@
         <f t="shared" si="2"/>
         <v>-9.61</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1</v>
       </c>
@@ -16359,8 +16883,11 @@
         <f t="shared" si="2"/>
         <v>-0.90000000000000568</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>1</v>
       </c>
@@ -16391,8 +16918,11 @@
         <f t="shared" si="2"/>
         <v>5.3099999999999952</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1</v>
       </c>
@@ -16420,8 +16950,11 @@
         <f t="shared" si="2"/>
         <v>1.4600000000000009</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1</v>
       </c>
@@ -16449,8 +16982,11 @@
         <f t="shared" si="2"/>
         <v>1.7899999999999991</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1</v>
       </c>
@@ -16481,8 +17017,11 @@
         <f t="shared" si="2"/>
         <v>6.7399999999999949</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1</v>
       </c>
@@ -16510,8 +17049,11 @@
         <f t="shared" si="2"/>
         <v>5.9699999999999989</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>1</v>
       </c>
@@ -16536,8 +17078,11 @@
         <f t="shared" si="2"/>
         <v>-36.96</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1</v>
       </c>
@@ -16565,8 +17110,11 @@
         <f t="shared" si="2"/>
         <v>4.0300000000000011</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>1</v>
       </c>
@@ -16597,8 +17145,11 @@
         <f t="shared" si="2"/>
         <v>2.8700000000000045</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>1</v>
       </c>
@@ -16629,8 +17180,11 @@
         <f t="shared" si="2"/>
         <v>5.5900000000000034</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>1</v>
       </c>
@@ -16658,8 +17212,11 @@
         <f t="shared" si="2"/>
         <v>0.29999999999999716</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>1</v>
       </c>
@@ -16687,8 +17244,11 @@
         <f t="shared" si="2"/>
         <v>2.2900000000000063</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>1</v>
       </c>
@@ -16716,8 +17276,11 @@
         <f t="shared" si="2"/>
         <v>3.6200000000000045</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>1</v>
       </c>
@@ -16742,8 +17305,11 @@
         <f t="shared" si="2"/>
         <v>-30.81</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>1</v>
       </c>
@@ -16771,8 +17337,11 @@
         <f t="shared" si="2"/>
         <v>2.0799999999999983</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>1</v>
       </c>
@@ -16803,8 +17372,11 @@
         <f t="shared" si="2"/>
         <v>-18.79</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>1</v>
       </c>
@@ -16832,8 +17404,11 @@
         <f t="shared" si="2"/>
         <v>-5.2700000000000031</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K185">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>1</v>
       </c>
@@ -16861,8 +17436,11 @@
         <f t="shared" si="2"/>
         <v>7.3500000000000014</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>1</v>
       </c>
@@ -16890,8 +17468,11 @@
         <f t="shared" si="2"/>
         <v>3.0700000000000003</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>1</v>
       </c>
@@ -16916,8 +17497,11 @@
         <f t="shared" si="2"/>
         <v>-36.44</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>1</v>
       </c>
@@ -16942,8 +17526,11 @@
         <f t="shared" si="2"/>
         <v>-26.44</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K189">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>1</v>
       </c>
@@ -16971,8 +17558,11 @@
         <f t="shared" si="2"/>
         <v>-11.299999999999997</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K190">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>1</v>
       </c>
@@ -17000,8 +17590,11 @@
         <f t="shared" si="2"/>
         <v>4.59</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>1</v>
       </c>
@@ -17026,8 +17619,11 @@
         <f t="shared" si="2"/>
         <v>-18.22</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>1</v>
       </c>
@@ -17055,8 +17651,11 @@
         <f t="shared" si="2"/>
         <v>10.299999999999997</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>1</v>
       </c>
@@ -17084,8 +17683,11 @@
         <f t="shared" si="2"/>
         <v>-2.3400000000000034</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>1</v>
       </c>
@@ -17116,8 +17718,11 @@
         <f t="shared" ref="J195:J258" si="3">I195-G195</f>
         <v>-2.7399999999999949</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>1</v>
       </c>
@@ -17142,8 +17747,11 @@
         <f t="shared" si="3"/>
         <v>-33.56</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>1</v>
       </c>
@@ -17171,8 +17779,11 @@
         <f t="shared" si="3"/>
         <v>-33.630000000000003</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K197">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>1</v>
       </c>
@@ -17200,8 +17811,11 @@
         <f t="shared" si="3"/>
         <v>-30.37</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>1</v>
       </c>
@@ -17229,8 +17843,11 @@
         <f t="shared" si="3"/>
         <v>0.57999999999999829</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>1</v>
       </c>
@@ -17255,8 +17872,11 @@
         <f t="shared" si="3"/>
         <v>-32.89</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>1</v>
       </c>
@@ -17281,8 +17901,11 @@
         <f t="shared" si="3"/>
         <v>-33.78</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1</v>
       </c>
@@ -17310,8 +17933,11 @@
         <f t="shared" si="3"/>
         <v>10.489999999999998</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K202">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1</v>
       </c>
@@ -17342,8 +17968,11 @@
         <f t="shared" si="3"/>
         <v>8.0600000000000023</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K203">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1</v>
       </c>
@@ -17371,8 +18000,11 @@
         <f t="shared" si="3"/>
         <v>3.1000000000000014</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K204">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1</v>
       </c>
@@ -17400,8 +18032,11 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K205">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1</v>
       </c>
@@ -17426,8 +18061,11 @@
         <f t="shared" si="3"/>
         <v>-30.07</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1</v>
       </c>
@@ -17452,8 +18090,11 @@
         <f t="shared" si="3"/>
         <v>-40.22</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>1</v>
       </c>
@@ -17478,8 +18119,11 @@
         <f t="shared" si="3"/>
         <v>-35.19</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1</v>
       </c>
@@ -17507,8 +18151,11 @@
         <f t="shared" si="3"/>
         <v>3.009999999999998</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K209">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>1</v>
       </c>
@@ -17536,8 +18183,11 @@
         <f t="shared" si="3"/>
         <v>3.259999999999998</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K210">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>1</v>
       </c>
@@ -17565,8 +18215,11 @@
         <f t="shared" si="3"/>
         <v>2.3399999999999963</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K211">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>1</v>
       </c>
@@ -17594,8 +18247,11 @@
         <f t="shared" si="3"/>
         <v>-0.92999999999999972</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>1</v>
       </c>
@@ -17626,8 +18282,11 @@
         <f t="shared" si="3"/>
         <v>-1.639999999999997</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>1</v>
       </c>
@@ -17658,8 +18317,11 @@
         <f t="shared" si="3"/>
         <v>5.7199999999999989</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1</v>
       </c>
@@ -17690,8 +18352,11 @@
         <f t="shared" si="3"/>
         <v>-5.0199999999999996</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1</v>
       </c>
@@ -17719,8 +18384,11 @@
         <f t="shared" si="3"/>
         <v>9.8299999999999983</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>1</v>
       </c>
@@ -17751,8 +18419,11 @@
         <f t="shared" si="3"/>
         <v>0.37000000000000099</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>1</v>
       </c>
@@ -17780,8 +18451,11 @@
         <f t="shared" si="3"/>
         <v>-5.43</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>1</v>
       </c>
@@ -17809,8 +18483,11 @@
         <f t="shared" si="3"/>
         <v>2.8500000000000014</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>1</v>
       </c>
@@ -17841,8 +18518,11 @@
         <f t="shared" si="3"/>
         <v>3.740000000000002</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>1</v>
       </c>
@@ -17873,8 +18553,11 @@
         <f t="shared" si="3"/>
         <v>4.5499999999999972</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>1</v>
       </c>
@@ -17902,8 +18585,11 @@
         <f t="shared" si="3"/>
         <v>-21.509999999999998</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>1</v>
       </c>
@@ -17931,8 +18617,11 @@
         <f t="shared" si="3"/>
         <v>10.239999999999998</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>1</v>
       </c>
@@ -17957,8 +18646,11 @@
         <f t="shared" si="3"/>
         <v>-25.93</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>1</v>
       </c>
@@ -17986,8 +18678,11 @@
         <f t="shared" si="3"/>
         <v>5.6899999999999977</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>1</v>
       </c>
@@ -18015,8 +18710,11 @@
         <f t="shared" si="3"/>
         <v>-36.520000000000003</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>1</v>
       </c>
@@ -18044,8 +18742,11 @@
         <f t="shared" si="3"/>
         <v>6.3699999999999974</v>
       </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>1</v>
       </c>
@@ -18076,8 +18777,11 @@
         <f t="shared" si="3"/>
         <v>4.4200000000000017</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>1</v>
       </c>
@@ -18105,8 +18809,11 @@
         <f t="shared" si="3"/>
         <v>1.6799999999999997</v>
       </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>1</v>
       </c>
@@ -18131,8 +18838,11 @@
         <f t="shared" si="3"/>
         <v>-30.96</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>1</v>
       </c>
@@ -18160,8 +18870,11 @@
         <f t="shared" si="3"/>
         <v>-8.5399999999999991</v>
       </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>1</v>
       </c>
@@ -18186,8 +18899,11 @@
         <f t="shared" si="3"/>
         <v>-30.96</v>
       </c>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>1</v>
       </c>
@@ -18215,8 +18931,11 @@
         <f t="shared" si="3"/>
         <v>-5.3200000000000038</v>
       </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>1</v>
       </c>
@@ -18244,8 +18963,11 @@
         <f t="shared" si="3"/>
         <v>3.8900000000000006</v>
       </c>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>1</v>
       </c>
@@ -18273,8 +18995,11 @@
         <f t="shared" si="3"/>
         <v>3.1099999999999994</v>
       </c>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>1</v>
       </c>
@@ -18305,8 +19030,11 @@
         <f t="shared" si="3"/>
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>1</v>
       </c>
@@ -18334,8 +19062,11 @@
         <f t="shared" si="3"/>
         <v>-1.0700000000000003</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>1</v>
       </c>
@@ -18360,8 +19091,11 @@
         <f t="shared" si="3"/>
         <v>-19.7</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>1</v>
       </c>
@@ -18389,8 +19123,11 @@
         <f t="shared" si="3"/>
         <v>8.5100000000000016</v>
       </c>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>1</v>
       </c>
@@ -18421,8 +19158,11 @@
         <f t="shared" si="3"/>
         <v>-0.27999999999999403</v>
       </c>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>1</v>
       </c>
@@ -18450,8 +19190,11 @@
         <f t="shared" si="3"/>
         <v>5.8599999999999994</v>
       </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>1</v>
       </c>
@@ -18476,8 +19219,11 @@
         <f t="shared" si="3"/>
         <v>-33.479999999999997</v>
       </c>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>1</v>
       </c>
@@ -18508,8 +19254,11 @@
         <f t="shared" si="3"/>
         <v>2.3599999999999994</v>
       </c>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K243">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>1</v>
       </c>
@@ -18540,8 +19289,11 @@
         <f t="shared" si="3"/>
         <v>0.58999999999999986</v>
       </c>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>1</v>
       </c>
@@ -18569,8 +19321,11 @@
         <f t="shared" si="3"/>
         <v>7.5399999999999991</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>1</v>
       </c>
@@ -18598,8 +19353,11 @@
         <f t="shared" si="3"/>
         <v>5.1899999999999977</v>
       </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>1</v>
       </c>
@@ -18627,8 +19385,11 @@
         <f t="shared" si="3"/>
         <v>0.42999999999999972</v>
       </c>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>1</v>
       </c>
@@ -18656,8 +19417,11 @@
         <f t="shared" si="3"/>
         <v>-6.1700000000000017</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>1</v>
       </c>
@@ -18688,8 +19452,11 @@
         <f t="shared" si="3"/>
         <v>3.9000000000000021</v>
       </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K249">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>1</v>
       </c>
@@ -18717,8 +19484,11 @@
         <f t="shared" si="3"/>
         <v>5.1499999999999986</v>
       </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K250">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>1</v>
       </c>
@@ -18746,8 +19516,11 @@
         <f t="shared" si="3"/>
         <v>-5.3699999999999974</v>
       </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>1</v>
       </c>
@@ -18775,8 +19548,11 @@
         <f t="shared" si="3"/>
         <v>10.260000000000005</v>
       </c>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K252">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>1</v>
       </c>
@@ -18804,8 +19580,11 @@
         <f t="shared" si="3"/>
         <v>-0.61999999999999744</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K253">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>1</v>
       </c>
@@ -18830,8 +19609,11 @@
         <f t="shared" si="3"/>
         <v>-27.19</v>
       </c>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K254">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>1</v>
       </c>
@@ -18856,8 +19638,11 @@
         <f t="shared" si="3"/>
         <v>-29.11</v>
       </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K255">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>1</v>
       </c>
@@ -18888,8 +19673,11 @@
         <f t="shared" si="3"/>
         <v>-24.159999999999997</v>
       </c>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K256">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>1</v>
       </c>
@@ -18914,8 +19702,11 @@
         <f t="shared" si="3"/>
         <v>-32.96</v>
       </c>
-    </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K257">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1</v>
       </c>
@@ -18943,8 +19734,11 @@
         <f t="shared" si="3"/>
         <v>3.2600000000000016</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K258">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1</v>
       </c>
@@ -18972,8 +19766,11 @@
         <f t="shared" ref="J259:J322" si="4">I259-G259</f>
         <v>19.71</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1</v>
       </c>
@@ -19004,8 +19801,11 @@
         <f t="shared" si="4"/>
         <v>11.52</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1</v>
       </c>
@@ -19033,8 +19833,11 @@
         <f t="shared" si="4"/>
         <v>-28.37</v>
       </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K261">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1</v>
       </c>
@@ -19062,8 +19865,11 @@
         <f t="shared" si="4"/>
         <v>8.1000000000000014</v>
       </c>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1</v>
       </c>
@@ -19094,8 +19900,11 @@
         <f t="shared" si="4"/>
         <v>5.629999999999999</v>
       </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K263">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1</v>
       </c>
@@ -19120,8 +19929,11 @@
         <f t="shared" si="4"/>
         <v>-32.07</v>
       </c>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1</v>
       </c>
@@ -19149,8 +19961,11 @@
         <f t="shared" si="4"/>
         <v>2.980000000000004</v>
       </c>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K265">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1</v>
       </c>
@@ -19178,8 +19993,11 @@
         <f t="shared" si="4"/>
         <v>-29.04</v>
       </c>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K266">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1</v>
       </c>
@@ -19207,8 +20025,11 @@
         <f t="shared" si="4"/>
         <v>9.0599999999999952</v>
       </c>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1</v>
       </c>
@@ -19236,8 +20057,11 @@
         <f t="shared" si="4"/>
         <v>-0.39999999999999858</v>
       </c>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K268">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1</v>
       </c>
@@ -19262,8 +20086,11 @@
         <f t="shared" si="4"/>
         <v>-31.78</v>
       </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1</v>
       </c>
@@ -19291,8 +20118,11 @@
         <f t="shared" si="4"/>
         <v>4.2700000000000031</v>
       </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K270">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1</v>
       </c>
@@ -19320,8 +20150,11 @@
         <f t="shared" si="4"/>
         <v>6.490000000000002</v>
       </c>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1</v>
       </c>
@@ -19349,8 +20182,11 @@
         <f t="shared" si="4"/>
         <v>2.3299999999999983</v>
       </c>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K272">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1</v>
       </c>
@@ -19375,8 +20211,11 @@
         <f t="shared" si="4"/>
         <v>-21.26</v>
       </c>
-    </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K273">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1</v>
       </c>
@@ -19401,8 +20240,11 @@
         <f t="shared" si="4"/>
         <v>-28.67</v>
       </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K274">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1</v>
       </c>
@@ -19427,8 +20269,11 @@
         <f t="shared" si="4"/>
         <v>-34.44</v>
       </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K275">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1</v>
       </c>
@@ -19459,8 +20304,11 @@
         <f t="shared" si="4"/>
         <v>-7.5500000000000007</v>
       </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K276">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1</v>
       </c>
@@ -19488,8 +20336,11 @@
         <f t="shared" si="4"/>
         <v>6.2199999999999989</v>
       </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1</v>
       </c>
@@ -19517,8 +20368,11 @@
         <f t="shared" si="4"/>
         <v>7.4699999999999989</v>
       </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K278">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1</v>
       </c>
@@ -19546,8 +20400,11 @@
         <f t="shared" si="4"/>
         <v>1.2399999999999984</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1</v>
       </c>
@@ -19575,8 +20432,11 @@
         <f t="shared" si="4"/>
         <v>10.86</v>
       </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1</v>
       </c>
@@ -19601,8 +20461,11 @@
         <f t="shared" si="4"/>
         <v>-28.44</v>
       </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1</v>
       </c>
@@ -19627,8 +20490,11 @@
         <f t="shared" si="4"/>
         <v>-32.74</v>
       </c>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1</v>
       </c>
@@ -19654,7 +20520,7 @@
         <v>-32.67</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1</v>
       </c>
@@ -19683,7 +20549,7 @@
         <v>-3.370000000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1</v>
       </c>
@@ -19709,7 +20575,7 @@
         <v>-31.41</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1</v>
       </c>
@@ -19741,7 +20607,7 @@
         <v>9.5100000000000051</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1</v>
       </c>
@@ -19770,7 +20636,7 @@
         <v>-0.51999999999999957</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1</v>
       </c>

</xml_diff>